<commit_message>
chore: auto-generate derived docs and explorer data
</commit_message>
<xml_diff>
--- a/docs/src/reference/data-dictionaries/S_Dict.xlsx
+++ b/docs/src/reference/data-dictionaries/S_Dict.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD204"/>
+  <dimension ref="A1:AD209"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10178,7 +10178,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Harm Reduction Policies</t>
+          <t>Buprenorphine Policy Proportion</t>
         </is>
       </c>
       <c r="C129" t="inlineStr"/>
@@ -10189,57 +10189,49 @@
       <c r="H129" t="inlineStr"/>
       <c r="I129" t="inlineStr"/>
       <c r="J129" t="inlineStr"/>
-      <c r="K129" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K129" t="inlineStr"/>
       <c r="L129" t="inlineStr"/>
-      <c r="M129" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="N129" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="O129" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="M129" t="inlineStr"/>
+      <c r="N129" t="inlineStr"/>
+      <c r="O129" t="inlineStr"/>
       <c r="P129" t="inlineStr"/>
-      <c r="Q129" t="inlineStr"/>
-      <c r="R129" t="inlineStr"/>
+      <c r="Q129" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="R129" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="S129" t="inlineStr"/>
       <c r="T129" t="inlineStr"/>
       <c r="U129" t="inlineStr"/>
       <c r="V129" t="inlineStr">
         <is>
-          <t>AnyGslDt</t>
+          <t>BupPolP</t>
         </is>
       </c>
       <c r="W129" t="inlineStr">
         <is>
-          <t>Any Good Samaritan Law (date)</t>
+          <t>Buprenorphine Policy Proportion</t>
         </is>
       </c>
       <c r="X129" t="inlineStr"/>
       <c r="Y129" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Good_Samaritan_Laws.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/medicaid_variables_saket/metadata/Bup_Policy_Proportion.md</t>
         </is>
       </c>
       <c r="Z129" t="inlineStr">
         <is>
-          <t>OPTIC 2017, 2019, 2020, 2021</t>
+          <t>CPHLR 2025</t>
         </is>
       </c>
       <c r="AA129" t="inlineStr">
         <is>
-          <t>RAND-USC Schaeffer Opioid Policy Tools and Information Center, 2017, 2019, 2020, 2021</t>
+          <t>Center for Public Health Law Research &amp; Vital Strategies</t>
         </is>
       </c>
       <c r="AB129" t="inlineStr"/>
@@ -10254,7 +10246,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Harm Reduction Policies</t>
+          <t>Buprenorphine Policy Proportion</t>
         </is>
       </c>
       <c r="C130" t="inlineStr"/>
@@ -10265,57 +10257,49 @@
       <c r="H130" t="inlineStr"/>
       <c r="I130" t="inlineStr"/>
       <c r="J130" t="inlineStr"/>
-      <c r="K130" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K130" t="inlineStr"/>
       <c r="L130" t="inlineStr"/>
-      <c r="M130" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="N130" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="O130" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="M130" t="inlineStr"/>
+      <c r="N130" t="inlineStr"/>
+      <c r="O130" t="inlineStr"/>
       <c r="P130" t="inlineStr"/>
-      <c r="Q130" t="inlineStr"/>
-      <c r="R130" t="inlineStr"/>
+      <c r="Q130" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="R130" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="S130" t="inlineStr"/>
       <c r="T130" t="inlineStr"/>
       <c r="U130" t="inlineStr"/>
       <c r="V130" t="inlineStr">
         <is>
-          <t>AnyGslFr</t>
+          <t>EdBupPolP</t>
         </is>
       </c>
       <c r="W130" t="inlineStr">
         <is>
-          <t>Any Good Samaritan Law (fraction of year in 2018)</t>
+          <t>Entire Data Period Buprenorphine Policy Proportion</t>
         </is>
       </c>
       <c r="X130" t="inlineStr"/>
       <c r="Y130" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Good_Samaritan_Laws.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/medicaid_variables_saket/metadata/Bup_Policy_Proportion.md</t>
         </is>
       </c>
       <c r="Z130" t="inlineStr">
         <is>
-          <t>OPTIC 2017, 2019, 2020, 2021</t>
+          <t>CPHLR 2025</t>
         </is>
       </c>
       <c r="AA130" t="inlineStr">
         <is>
-          <t>RAND-USC Schaeffer Opioid Policy Tools and Information Center, 2017, 2019, 2020, 2021</t>
+          <t>Center for Public Health Law Research &amp; Vital Strategies</t>
         </is>
       </c>
       <c r="AB130" t="inlineStr"/>
@@ -10330,7 +10314,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Harm Reduction Policies</t>
+          <t>Buprenorphine Policy Proportion</t>
         </is>
       </c>
       <c r="C131" t="inlineStr"/>
@@ -10341,65 +10325,49 @@
       <c r="H131" t="inlineStr"/>
       <c r="I131" t="inlineStr"/>
       <c r="J131" t="inlineStr"/>
-      <c r="K131" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="L131" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="M131" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="N131" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="O131" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="P131" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="Q131" t="inlineStr"/>
-      <c r="R131" t="inlineStr"/>
+      <c r="K131" t="inlineStr"/>
+      <c r="L131" t="inlineStr"/>
+      <c r="M131" t="inlineStr"/>
+      <c r="N131" t="inlineStr"/>
+      <c r="O131" t="inlineStr"/>
+      <c r="P131" t="inlineStr"/>
+      <c r="Q131" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="R131" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="S131" t="inlineStr"/>
       <c r="T131" t="inlineStr"/>
       <c r="U131" t="inlineStr"/>
       <c r="V131" t="inlineStr">
         <is>
-          <t>AnyNalxDt</t>
+          <t>PerImpBupP</t>
         </is>
       </c>
       <c r="W131" t="inlineStr">
         <is>
-          <t>Any Naloxone Law (date)</t>
+          <t>Periods of Buprenorphine Policy Implementation</t>
         </is>
       </c>
       <c r="X131" t="inlineStr"/>
       <c r="Y131" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Naloxone_Policy.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/medicaid_variables_saket/metadata/Bup_Policy_Proportion.md</t>
         </is>
       </c>
       <c r="Z131" t="inlineStr">
         <is>
-          <t>OPTIC 2017-2022</t>
+          <t>CPHLR 2025</t>
         </is>
       </c>
       <c r="AA131" t="inlineStr">
         <is>
-          <t>RAND-USC Schaeffer Opioid Policy Tools and Information Center, 2017-2022</t>
+          <t>Center for Public Health Law Research &amp; Vital Strategies</t>
         </is>
       </c>
       <c r="AB131" t="inlineStr"/>
@@ -10430,11 +10398,7 @@
           <t>x</t>
         </is>
       </c>
-      <c r="L132" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="L132" t="inlineStr"/>
       <c r="M132" t="inlineStr">
         <is>
           <t>x</t>
@@ -10450,11 +10414,7 @@
           <t>x</t>
         </is>
       </c>
-      <c r="P132" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P132" t="inlineStr"/>
       <c r="Q132" t="inlineStr"/>
       <c r="R132" t="inlineStr"/>
       <c r="S132" t="inlineStr"/>
@@ -10462,28 +10422,28 @@
       <c r="U132" t="inlineStr"/>
       <c r="V132" t="inlineStr">
         <is>
-          <t>AnyNalxFr</t>
+          <t>AnyGslDt</t>
         </is>
       </c>
       <c r="W132" t="inlineStr">
         <is>
-          <t>Naloxone Law allowing distribution through a standing or order (fraction of year in 2017)</t>
+          <t>Any Good Samaritan Law (date)</t>
         </is>
       </c>
       <c r="X132" t="inlineStr"/>
       <c r="Y132" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Naloxone_Policy.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Good_Samaritan_Laws.md</t>
         </is>
       </c>
       <c r="Z132" t="inlineStr">
         <is>
-          <t>OPTIC 2017-2022</t>
+          <t>OPTIC 2017, 2019, 2020, 2021</t>
         </is>
       </c>
       <c r="AA132" t="inlineStr">
         <is>
-          <t>RAND-USC Schaeffer Opioid Policy Tools and Information Center, 2017-2022</t>
+          <t>RAND-USC Schaeffer Opioid Policy Tools and Information Center, 2017, 2019, 2020, 2021</t>
         </is>
       </c>
       <c r="AB132" t="inlineStr"/>
@@ -10509,15 +10469,27 @@
       <c r="H133" t="inlineStr"/>
       <c r="I133" t="inlineStr"/>
       <c r="J133" t="inlineStr"/>
-      <c r="K133" t="inlineStr"/>
+      <c r="K133" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L133" t="inlineStr"/>
       <c r="M133" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="N133" t="inlineStr"/>
-      <c r="O133" t="inlineStr"/>
+      <c r="N133" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="O133" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="P133" t="inlineStr"/>
       <c r="Q133" t="inlineStr"/>
       <c r="R133" t="inlineStr"/>
@@ -10526,28 +10498,28 @@
       <c r="U133" t="inlineStr"/>
       <c r="V133" t="inlineStr">
         <is>
-          <t>ExpSsp</t>
+          <t>AnyGslFr</t>
         </is>
       </c>
       <c r="W133" t="inlineStr">
         <is>
-          <t>Syringe Service Program (SSP) Authorization Laws</t>
+          <t>Any Good Samaritan Law (fraction of year in 2018)</t>
         </is>
       </c>
       <c r="X133" t="inlineStr"/>
       <c r="Y133" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Syringe_Policy.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Good_Samaritan_Laws.md</t>
         </is>
       </c>
       <c r="Z133" t="inlineStr">
         <is>
-          <t>LawAtlas 2019</t>
+          <t>OPTIC 2017, 2019, 2020, 2021</t>
         </is>
       </c>
       <c r="AA133" t="inlineStr">
         <is>
-          <t>Fernández-Viña MH, Prood NE, Herpolsheimer A, Waimberg J, Burris S. State Laws Governing Syringe Services Programs and Participant Syringe Possession, 2014-2019. Public Health Reports. 2020;135:128S-137S. doi:10.1177/0033354920921817</t>
+          <t>RAND-USC Schaeffer Opioid Policy Tools and Information Center, 2017, 2019, 2020, 2021</t>
         </is>
       </c>
       <c r="AB133" t="inlineStr"/>
@@ -10578,7 +10550,11 @@
           <t>x</t>
         </is>
       </c>
-      <c r="L134" t="inlineStr"/>
+      <c r="L134" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="M134" t="inlineStr">
         <is>
           <t>x</t>
@@ -10594,7 +10570,11 @@
           <t>x</t>
         </is>
       </c>
-      <c r="P134" t="inlineStr"/>
+      <c r="P134" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q134" t="inlineStr"/>
       <c r="R134" t="inlineStr"/>
       <c r="S134" t="inlineStr"/>
@@ -10602,28 +10582,28 @@
       <c r="U134" t="inlineStr"/>
       <c r="V134" t="inlineStr">
         <is>
-          <t>GslArrDt</t>
+          <t>AnyNalxDt</t>
         </is>
       </c>
       <c r="W134" t="inlineStr">
         <is>
-          <t>Good Samaritan Law Protecting Arrest (date)</t>
+          <t>Any Naloxone Law (date)</t>
         </is>
       </c>
       <c r="X134" t="inlineStr"/>
       <c r="Y134" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Good_Samaritan_Laws.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Naloxone_Policy.md</t>
         </is>
       </c>
       <c r="Z134" t="inlineStr">
         <is>
-          <t>OPTIC 2017, 2019, 2020, 2021</t>
+          <t>OPTIC 2017-2022</t>
         </is>
       </c>
       <c r="AA134" t="inlineStr">
         <is>
-          <t>RAND-USC Schaeffer Opioid Policy Tools and Information Center, 2017, 2019, 2020, 2021</t>
+          <t>RAND-USC Schaeffer Opioid Policy Tools and Information Center, 2017-2022</t>
         </is>
       </c>
       <c r="AB134" t="inlineStr"/>
@@ -10654,7 +10634,11 @@
           <t>x</t>
         </is>
       </c>
-      <c r="L135" t="inlineStr"/>
+      <c r="L135" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="M135" t="inlineStr">
         <is>
           <t>x</t>
@@ -10670,7 +10654,11 @@
           <t>x</t>
         </is>
       </c>
-      <c r="P135" t="inlineStr"/>
+      <c r="P135" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q135" t="inlineStr"/>
       <c r="R135" t="inlineStr"/>
       <c r="S135" t="inlineStr"/>
@@ -10678,28 +10666,28 @@
       <c r="U135" t="inlineStr"/>
       <c r="V135" t="inlineStr">
         <is>
-          <t>GslArrFr</t>
+          <t>AnyNalxFr</t>
         </is>
       </c>
       <c r="W135" t="inlineStr">
         <is>
-          <t>Good Samaritan Law Protecting Arrest (fraction of year in 2018)</t>
+          <t>Naloxone Law allowing distribution through a standing or order (fraction of year in 2017)</t>
         </is>
       </c>
       <c r="X135" t="inlineStr"/>
       <c r="Y135" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Good_Samaritan_Laws.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Naloxone_Policy.md</t>
         </is>
       </c>
       <c r="Z135" t="inlineStr">
         <is>
-          <t>OPTIC 2017, 2019, 2020, 2021</t>
+          <t>OPTIC 2017-2022</t>
         </is>
       </c>
       <c r="AA135" t="inlineStr">
         <is>
-          <t>RAND-USC Schaeffer Opioid Policy Tools and Information Center, 2017, 2019, 2020, 2021</t>
+          <t>RAND-USC Schaeffer Opioid Policy Tools and Information Center, 2017-2022</t>
         </is>
       </c>
       <c r="AB135" t="inlineStr"/>
@@ -10725,36 +10713,16 @@
       <c r="H136" t="inlineStr"/>
       <c r="I136" t="inlineStr"/>
       <c r="J136" t="inlineStr"/>
-      <c r="K136" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="L136" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K136" t="inlineStr"/>
+      <c r="L136" t="inlineStr"/>
       <c r="M136" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="N136" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="O136" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="P136" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="N136" t="inlineStr"/>
+      <c r="O136" t="inlineStr"/>
+      <c r="P136" t="inlineStr"/>
       <c r="Q136" t="inlineStr"/>
       <c r="R136" t="inlineStr"/>
       <c r="S136" t="inlineStr"/>
@@ -10762,28 +10730,28 @@
       <c r="U136" t="inlineStr"/>
       <c r="V136" t="inlineStr">
         <is>
-          <t>NalxPrStDt</t>
+          <t>ExpSsp</t>
         </is>
       </c>
       <c r="W136" t="inlineStr">
         <is>
-          <t>Naloxone Law allowing distribution through a standing or order (date)</t>
+          <t>Syringe Service Program (SSP) Authorization Laws</t>
         </is>
       </c>
       <c r="X136" t="inlineStr"/>
       <c r="Y136" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Naloxone_Policy.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Syringe_Policy.md</t>
         </is>
       </c>
       <c r="Z136" t="inlineStr">
         <is>
-          <t>OPTIC 2017-2022</t>
+          <t>LawAtlas 2019</t>
         </is>
       </c>
       <c r="AA136" t="inlineStr">
         <is>
-          <t>RAND-USC Schaeffer Opioid Policy Tools and Information Center, 2017-2022</t>
+          <t>Fernández-Viña MH, Prood NE, Herpolsheimer A, Waimberg J, Burris S. State Laws Governing Syringe Services Programs and Participant Syringe Possession, 2014-2019. Public Health Reports. 2020;135:128S-137S. doi:10.1177/0033354920921817</t>
         </is>
       </c>
       <c r="AB136" t="inlineStr"/>
@@ -10814,11 +10782,7 @@
           <t>x</t>
         </is>
       </c>
-      <c r="L137" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="L137" t="inlineStr"/>
       <c r="M137" t="inlineStr">
         <is>
           <t>x</t>
@@ -10834,11 +10798,7 @@
           <t>x</t>
         </is>
       </c>
-      <c r="P137" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P137" t="inlineStr"/>
       <c r="Q137" t="inlineStr"/>
       <c r="R137" t="inlineStr"/>
       <c r="S137" t="inlineStr"/>
@@ -10846,28 +10806,28 @@
       <c r="U137" t="inlineStr"/>
       <c r="V137" t="inlineStr">
         <is>
-          <t>NalxPrStFr</t>
+          <t>GslArrDt</t>
         </is>
       </c>
       <c r="W137" t="inlineStr">
         <is>
-          <t>Naloxone Law in Effect (fraction of year in 2017)</t>
+          <t>Good Samaritan Law Protecting Arrest (date)</t>
         </is>
       </c>
       <c r="X137" t="inlineStr"/>
       <c r="Y137" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Naloxone_Policy.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Good_Samaritan_Laws.md</t>
         </is>
       </c>
       <c r="Z137" t="inlineStr">
         <is>
-          <t>OPTIC 2017-2022</t>
+          <t>OPTIC 2017, 2019, 2020, 2021</t>
         </is>
       </c>
       <c r="AA137" t="inlineStr">
         <is>
-          <t>RAND-USC Schaeffer Opioid Policy Tools and Information Center, 2017-2022</t>
+          <t>RAND-USC Schaeffer Opioid Policy Tools and Information Center, 2017, 2019, 2020, 2021</t>
         </is>
       </c>
       <c r="AB137" t="inlineStr"/>
@@ -10898,11 +10858,7 @@
           <t>x</t>
         </is>
       </c>
-      <c r="L138" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="L138" t="inlineStr"/>
       <c r="M138" t="inlineStr">
         <is>
           <t>x</t>
@@ -10918,11 +10874,7 @@
           <t>x</t>
         </is>
       </c>
-      <c r="P138" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P138" t="inlineStr"/>
       <c r="Q138" t="inlineStr"/>
       <c r="R138" t="inlineStr"/>
       <c r="S138" t="inlineStr"/>
@@ -10930,28 +10882,28 @@
       <c r="U138" t="inlineStr"/>
       <c r="V138" t="inlineStr">
         <is>
-          <t>NalxPresDt</t>
+          <t>GslArrFr</t>
         </is>
       </c>
       <c r="W138" t="inlineStr">
         <is>
-          <t>Naloxone Law allowing pharmacists prescriptive authority (date)</t>
+          <t>Good Samaritan Law Protecting Arrest (fraction of year in 2018)</t>
         </is>
       </c>
       <c r="X138" t="inlineStr"/>
       <c r="Y138" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Naloxone_Policy.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Good_Samaritan_Laws.md</t>
         </is>
       </c>
       <c r="Z138" t="inlineStr">
         <is>
-          <t>OPTIC 2017-2022</t>
+          <t>OPTIC 2017, 2019, 2020, 2021</t>
         </is>
       </c>
       <c r="AA138" t="inlineStr">
         <is>
-          <t>RAND-USC Schaeffer Opioid Policy Tools and Information Center, 2017-2022</t>
+          <t>RAND-USC Schaeffer Opioid Policy Tools and Information Center, 2017, 2019, 2020, 2021</t>
         </is>
       </c>
       <c r="AB138" t="inlineStr"/>
@@ -11014,12 +10966,12 @@
       <c r="U139" t="inlineStr"/>
       <c r="V139" t="inlineStr">
         <is>
-          <t>NalxPresFr</t>
+          <t>NalxPrStDt</t>
         </is>
       </c>
       <c r="W139" t="inlineStr">
         <is>
-          <t>Naloxone Law allowing pharmacists prescriptive authority (fraction of year in 2017)</t>
+          <t>Naloxone Law allowing distribution through a standing or order (date)</t>
         </is>
       </c>
       <c r="X139" t="inlineStr"/>
@@ -11061,16 +11013,36 @@
       <c r="H140" t="inlineStr"/>
       <c r="I140" t="inlineStr"/>
       <c r="J140" t="inlineStr"/>
-      <c r="K140" t="inlineStr"/>
-      <c r="L140" t="inlineStr"/>
+      <c r="K140" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="L140" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="M140" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="N140" t="inlineStr"/>
-      <c r="O140" t="inlineStr"/>
-      <c r="P140" t="inlineStr"/>
+      <c r="N140" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="O140" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="P140" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q140" t="inlineStr"/>
       <c r="R140" t="inlineStr"/>
       <c r="S140" t="inlineStr"/>
@@ -11078,28 +11050,28 @@
       <c r="U140" t="inlineStr"/>
       <c r="V140" t="inlineStr">
         <is>
-          <t>NoLwRmUnc</t>
+          <t>NalxPrStFr</t>
         </is>
       </c>
       <c r="W140" t="inlineStr">
         <is>
-          <t>Laws removing barriers to SSPs</t>
+          <t>Naloxone Law in Effect (fraction of year in 2017)</t>
         </is>
       </c>
       <c r="X140" t="inlineStr"/>
       <c r="Y140" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Syringe_Policy.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Naloxone_Policy.md</t>
         </is>
       </c>
       <c r="Z140" t="inlineStr">
         <is>
-          <t>LawAtlas 2019</t>
+          <t>OPTIC 2017-2022</t>
         </is>
       </c>
       <c r="AA140" t="inlineStr">
         <is>
-          <t>Fernández-Viña MH, Prood NE, Herpolsheimer A, Waimberg J, Burris S. State Laws Governing Syringe Services Programs and Participant Syringe Possession, 2014-2019. Public Health Reports. 2020;135:128S-137S. doi:10.1177/0033354920921817</t>
+          <t>RAND-USC Schaeffer Opioid Policy Tools and Information Center, 2017-2022</t>
         </is>
       </c>
       <c r="AB140" t="inlineStr"/>
@@ -11125,16 +11097,36 @@
       <c r="H141" t="inlineStr"/>
       <c r="I141" t="inlineStr"/>
       <c r="J141" t="inlineStr"/>
-      <c r="K141" t="inlineStr"/>
-      <c r="L141" t="inlineStr"/>
+      <c r="K141" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="L141" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="M141" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="N141" t="inlineStr"/>
-      <c r="O141" t="inlineStr"/>
-      <c r="P141" t="inlineStr"/>
+      <c r="N141" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="O141" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="P141" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q141" t="inlineStr"/>
       <c r="R141" t="inlineStr"/>
       <c r="S141" t="inlineStr"/>
@@ -11142,28 +11134,28 @@
       <c r="U141" t="inlineStr"/>
       <c r="V141" t="inlineStr">
         <is>
-          <t>NoPrphLw</t>
+          <t>NalxPresDt</t>
         </is>
       </c>
       <c r="W141" t="inlineStr">
         <is>
-          <t>Drug Paraphernalia Laws</t>
+          <t>Naloxone Law allowing pharmacists prescriptive authority (date)</t>
         </is>
       </c>
       <c r="X141" t="inlineStr"/>
       <c r="Y141" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Syringe_Policy.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Naloxone_Policy.md</t>
         </is>
       </c>
       <c r="Z141" t="inlineStr">
         <is>
-          <t>LawAtlas 2019</t>
+          <t>OPTIC 2017-2022</t>
         </is>
       </c>
       <c r="AA141" t="inlineStr">
         <is>
-          <t>Fernández-Viña MH, Prood NE, Herpolsheimer A, Waimberg J, Burris S. State Laws Governing Syringe Services Programs and Participant Syringe Possession, 2014-2019. Public Health Reports. 2020;135:128S-137S. doi:10.1177/0033354920921817</t>
+          <t>RAND-USC Schaeffer Opioid Policy Tools and Information Center, 2017-2022</t>
         </is>
       </c>
       <c r="AB141" t="inlineStr"/>
@@ -11189,16 +11181,36 @@
       <c r="H142" t="inlineStr"/>
       <c r="I142" t="inlineStr"/>
       <c r="J142" t="inlineStr"/>
-      <c r="K142" t="inlineStr"/>
-      <c r="L142" t="inlineStr"/>
+      <c r="K142" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="L142" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="M142" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="N142" t="inlineStr"/>
-      <c r="O142" t="inlineStr"/>
-      <c r="P142" t="inlineStr"/>
+      <c r="N142" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="O142" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="P142" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q142" t="inlineStr"/>
       <c r="R142" t="inlineStr"/>
       <c r="S142" t="inlineStr"/>
@@ -11206,28 +11218,28 @@
       <c r="U142" t="inlineStr"/>
       <c r="V142" t="inlineStr">
         <is>
-          <t>NtPrFrDsSy</t>
+          <t>NalxPresFr</t>
         </is>
       </c>
       <c r="W142" t="inlineStr">
         <is>
-          <t>Distribution of Syringes Laws</t>
+          <t>Naloxone Law allowing pharmacists prescriptive authority (fraction of year in 2017)</t>
         </is>
       </c>
       <c r="X142" t="inlineStr"/>
       <c r="Y142" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Syringe_Policy.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Naloxone_Policy.md</t>
         </is>
       </c>
       <c r="Z142" t="inlineStr">
         <is>
-          <t>LawAtlas 2019</t>
+          <t>OPTIC 2017-2022</t>
         </is>
       </c>
       <c r="AA142" t="inlineStr">
         <is>
-          <t>Fernández-Viña MH, Prood NE, Herpolsheimer A, Waimberg J, Burris S. State Laws Governing Syringe Services Programs and Participant Syringe Possession, 2014-2019. Public Health Reports. 2020;135:128S-137S. doi:10.1177/0033354920921817</t>
+          <t>RAND-USC Schaeffer Opioid Policy Tools and Information Center, 2017-2022</t>
         </is>
       </c>
       <c r="AB142" t="inlineStr"/>
@@ -11270,12 +11282,12 @@
       <c r="U143" t="inlineStr"/>
       <c r="V143" t="inlineStr">
         <is>
-          <t>PrExcInj</t>
+          <t>NoLwRmUnc</t>
         </is>
       </c>
       <c r="W143" t="inlineStr">
         <is>
-          <t>Paraphernalia exludes objects used for injecting drugs</t>
+          <t>Laws removing barriers to SSPs</t>
         </is>
       </c>
       <c r="X143" t="inlineStr"/>
@@ -11334,12 +11346,12 @@
       <c r="U144" t="inlineStr"/>
       <c r="V144" t="inlineStr">
         <is>
-          <t>PrNtRefInj</t>
+          <t>NoPrphLw</t>
         </is>
       </c>
       <c r="W144" t="inlineStr">
         <is>
-          <t>Paraphernalia does not refer to objects used for injecting drugs</t>
+          <t>Drug Paraphernalia Laws</t>
         </is>
       </c>
       <c r="X144" t="inlineStr"/>
@@ -11370,7 +11382,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Marijuana Policies</t>
+          <t>Harm Reduction Policies</t>
         </is>
       </c>
       <c r="C145" t="inlineStr"/>
@@ -11381,69 +11393,45 @@
       <c r="H145" t="inlineStr"/>
       <c r="I145" t="inlineStr"/>
       <c r="J145" t="inlineStr"/>
-      <c r="K145" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="L145" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K145" t="inlineStr"/>
+      <c r="L145" t="inlineStr"/>
       <c r="M145" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="N145" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="O145" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="P145" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="Q145" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="N145" t="inlineStr"/>
+      <c r="O145" t="inlineStr"/>
+      <c r="P145" t="inlineStr"/>
+      <c r="Q145" t="inlineStr"/>
       <c r="R145" t="inlineStr"/>
       <c r="S145" t="inlineStr"/>
       <c r="T145" t="inlineStr"/>
       <c r="U145" t="inlineStr"/>
       <c r="V145" t="inlineStr">
         <is>
-          <t>MdMarijLaw</t>
+          <t>NtPrFrDsSy</t>
         </is>
       </c>
       <c r="W145" t="inlineStr">
         <is>
-          <t xml:space="preserve">Laws authorizing medical marijuana use </t>
+          <t>Distribution of Syringes Laws</t>
         </is>
       </c>
       <c r="X145" t="inlineStr"/>
       <c r="Y145" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Medical_Marijuana_Laws.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Syringe_Policy.md</t>
         </is>
       </c>
       <c r="Z145" t="inlineStr">
         <is>
-          <t>PDAPS 2017</t>
+          <t>LawAtlas 2019</t>
         </is>
       </c>
       <c r="AA145" t="inlineStr">
         <is>
-          <t>Prescription Drug Abuse Policy System, Medical Marijuana Caregiver Rules, 2017</t>
+          <t>Fernández-Viña MH, Prood NE, Herpolsheimer A, Waimberg J, Burris S. State Laws Governing Syringe Services Programs and Participant Syringe Possession, 2014-2019. Public Health Reports. 2020;135:128S-137S. doi:10.1177/0033354920921817</t>
         </is>
       </c>
       <c r="AB145" t="inlineStr"/>
@@ -11458,7 +11446,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Prescription Drug Monitoring Programs (PDMP)</t>
+          <t>Harm Reduction Policies</t>
         </is>
       </c>
       <c r="C146" t="inlineStr"/>
@@ -11469,69 +11457,45 @@
       <c r="H146" t="inlineStr"/>
       <c r="I146" t="inlineStr"/>
       <c r="J146" t="inlineStr"/>
-      <c r="K146" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="L146" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K146" t="inlineStr"/>
+      <c r="L146" t="inlineStr"/>
       <c r="M146" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="N146" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="O146" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="P146" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="Q146" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="N146" t="inlineStr"/>
+      <c r="O146" t="inlineStr"/>
+      <c r="P146" t="inlineStr"/>
+      <c r="Q146" t="inlineStr"/>
       <c r="R146" t="inlineStr"/>
       <c r="S146" t="inlineStr"/>
       <c r="T146" t="inlineStr"/>
       <c r="U146" t="inlineStr"/>
       <c r="V146" t="inlineStr">
         <is>
-          <t>AnyPdmpDt</t>
+          <t>PrExcInj</t>
         </is>
       </c>
       <c r="W146" t="inlineStr">
         <is>
-          <t>Any PDMP start date</t>
+          <t>Paraphernalia exludes objects used for injecting drugs</t>
         </is>
       </c>
       <c r="X146" t="inlineStr"/>
       <c r="Y146" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/PDMP_Presence.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Syringe_Policy.md</t>
         </is>
       </c>
       <c r="Z146" t="inlineStr">
         <is>
-          <t>OPTIC 2017-2022</t>
+          <t>LawAtlas 2019</t>
         </is>
       </c>
       <c r="AA146" t="inlineStr">
         <is>
-          <t>RAND-USC Schaeffer Opioid Policy Tools and Information Center, 2017-2022</t>
+          <t>Fernández-Viña MH, Prood NE, Herpolsheimer A, Waimberg J, Burris S. State Laws Governing Syringe Services Programs and Participant Syringe Possession, 2014-2019. Public Health Reports. 2020;135:128S-137S. doi:10.1177/0033354920921817</t>
         </is>
       </c>
       <c r="AB146" t="inlineStr"/>
@@ -11546,7 +11510,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Prescription Drug Monitoring Programs (PDMP)</t>
+          <t>Harm Reduction Policies</t>
         </is>
       </c>
       <c r="C147" t="inlineStr"/>
@@ -11557,69 +11521,45 @@
       <c r="H147" t="inlineStr"/>
       <c r="I147" t="inlineStr"/>
       <c r="J147" t="inlineStr"/>
-      <c r="K147" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="L147" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K147" t="inlineStr"/>
+      <c r="L147" t="inlineStr"/>
       <c r="M147" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="N147" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="O147" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="P147" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="Q147" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="N147" t="inlineStr"/>
+      <c r="O147" t="inlineStr"/>
+      <c r="P147" t="inlineStr"/>
+      <c r="Q147" t="inlineStr"/>
       <c r="R147" t="inlineStr"/>
       <c r="S147" t="inlineStr"/>
       <c r="T147" t="inlineStr"/>
       <c r="U147" t="inlineStr"/>
       <c r="V147" t="inlineStr">
         <is>
-          <t>AnyPdmpFr</t>
+          <t>PrNtRefInj</t>
         </is>
       </c>
       <c r="W147" t="inlineStr">
         <is>
-          <t>Any PDMP (fraction of year in 2017)</t>
+          <t>Paraphernalia does not refer to objects used for injecting drugs</t>
         </is>
       </c>
       <c r="X147" t="inlineStr"/>
       <c r="Y147" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/PDMP_Presence.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Syringe_Policy.md</t>
         </is>
       </c>
       <c r="Z147" t="inlineStr">
         <is>
-          <t>OPTIC 2017-2022</t>
+          <t>LawAtlas 2019</t>
         </is>
       </c>
       <c r="AA147" t="inlineStr">
         <is>
-          <t>RAND-USC Schaeffer Opioid Policy Tools and Information Center, 2017-2022</t>
+          <t>Fernández-Viña MH, Prood NE, Herpolsheimer A, Waimberg J, Burris S. State Laws Governing Syringe Services Programs and Participant Syringe Possession, 2014-2019. Public Health Reports. 2020;135:128S-137S. doi:10.1177/0033354920921817</t>
         </is>
       </c>
       <c r="AB147" t="inlineStr"/>
@@ -11634,7 +11574,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Prescription Drug Monitoring Programs (PDMP)</t>
+          <t>Marijuana Policies</t>
         </is>
       </c>
       <c r="C148" t="inlineStr"/>
@@ -11686,28 +11626,28 @@
       <c r="U148" t="inlineStr"/>
       <c r="V148" t="inlineStr">
         <is>
-          <t>AnyPdmphDt</t>
+          <t>MdMarijLaw</t>
         </is>
       </c>
       <c r="W148" t="inlineStr">
         <is>
-          <t>Any Horowitz PDMP start date</t>
+          <t xml:space="preserve">Laws authorizing medical marijuana use </t>
         </is>
       </c>
       <c r="X148" t="inlineStr"/>
       <c r="Y148" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/PDMP_Presence.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Medical_Marijuana_Laws.md</t>
         </is>
       </c>
       <c r="Z148" t="inlineStr">
         <is>
-          <t>OPTIC 2017-2022</t>
+          <t>PDAPS 2017</t>
         </is>
       </c>
       <c r="AA148" t="inlineStr">
         <is>
-          <t>RAND-USC Schaeffer Opioid Policy Tools and Information Center, 2017-2022</t>
+          <t>Prescription Drug Abuse Policy System, Medical Marijuana Caregiver Rules, 2017</t>
         </is>
       </c>
       <c r="AB148" t="inlineStr"/>
@@ -11722,7 +11662,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Prescription Drug Monitoring Programs (PDMP)</t>
+          <t>Medicaid Policy Proportion</t>
         </is>
       </c>
       <c r="C149" t="inlineStr"/>
@@ -11733,69 +11673,49 @@
       <c r="H149" t="inlineStr"/>
       <c r="I149" t="inlineStr"/>
       <c r="J149" t="inlineStr"/>
-      <c r="K149" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="L149" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K149" t="inlineStr"/>
+      <c r="L149" t="inlineStr"/>
       <c r="M149" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="N149" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="O149" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="P149" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="Q149" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="R149" t="inlineStr"/>
+      <c r="N149" t="inlineStr"/>
+      <c r="O149" t="inlineStr"/>
+      <c r="P149" t="inlineStr"/>
+      <c r="Q149" t="inlineStr"/>
+      <c r="R149" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="S149" t="inlineStr"/>
       <c r="T149" t="inlineStr"/>
       <c r="U149" t="inlineStr"/>
       <c r="V149" t="inlineStr">
         <is>
-          <t>AnyPdmphFr</t>
+          <t>MedPolP5Yr</t>
         </is>
       </c>
       <c r="W149" t="inlineStr">
         <is>
-          <t>Any Horowitz PDMP (fraction of year in 2017)</t>
+          <t>Five-Year Medicaid Expansion Proportion</t>
         </is>
       </c>
       <c r="X149" t="inlineStr"/>
       <c r="Y149" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/PDMP_Presence.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/medicaid_variables_saket/metadata/Medicaid_Policy_Proportion.md</t>
         </is>
       </c>
       <c r="Z149" t="inlineStr">
         <is>
-          <t>OPTIC 2017-2022</t>
+          <t>KFF 2025</t>
         </is>
       </c>
       <c r="AA149" t="inlineStr">
         <is>
-          <t>RAND-USC Schaeffer Opioid Policy Tools and Information Center, 2017-2022</t>
+          <t>KFF (Status of State Action on Medicaid Expansion Decision) 2025</t>
         </is>
       </c>
       <c r="AB149" t="inlineStr"/>
@@ -11810,7 +11730,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Prescription Drug Monitoring Programs (PDMP)</t>
+          <t>Medicaid Policy Proportion</t>
         </is>
       </c>
       <c r="C150" t="inlineStr"/>
@@ -11818,9 +11738,21 @@
       <c r="E150" t="inlineStr"/>
       <c r="F150" t="inlineStr"/>
       <c r="G150" t="inlineStr"/>
-      <c r="H150" t="inlineStr"/>
-      <c r="I150" t="inlineStr"/>
-      <c r="J150" t="inlineStr"/>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="I150" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="J150" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="K150" t="inlineStr">
         <is>
           <t>x</t>
@@ -11856,34 +11788,38 @@
           <t>x</t>
         </is>
       </c>
-      <c r="R150" t="inlineStr"/>
+      <c r="R150" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="S150" t="inlineStr"/>
       <c r="T150" t="inlineStr"/>
       <c r="U150" t="inlineStr"/>
       <c r="V150" t="inlineStr">
         <is>
-          <t>ElcPdmpDt</t>
+          <t>MedPolProp</t>
         </is>
       </c>
       <c r="W150" t="inlineStr">
         <is>
-          <t>Electronic PDMP start date</t>
+          <t>Medicaid Expansion Proportion</t>
         </is>
       </c>
       <c r="X150" t="inlineStr"/>
       <c r="Y150" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/PDMP_Presence.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/medicaid_variables_saket/metadata/Medicaid_Policy_Proportion.md</t>
         </is>
       </c>
       <c r="Z150" t="inlineStr">
         <is>
-          <t>OPTIC 2017-2022</t>
+          <t>KFF 2025</t>
         </is>
       </c>
       <c r="AA150" t="inlineStr">
         <is>
-          <t>RAND-USC Schaeffer Opioid Policy Tools and Information Center, 2017-2022</t>
+          <t>KFF (Status of State Action on Medicaid Expansion Decision) 2025</t>
         </is>
       </c>
       <c r="AB150" t="inlineStr"/>
@@ -11950,12 +11886,12 @@
       <c r="U151" t="inlineStr"/>
       <c r="V151" t="inlineStr">
         <is>
-          <t>ElcPdmpFr</t>
+          <t>AnyPdmpDt</t>
         </is>
       </c>
       <c r="W151" t="inlineStr">
         <is>
-          <t>Electronic PDMP (fraction of year in 2017)</t>
+          <t>Any PDMP start date</t>
         </is>
       </c>
       <c r="X151" t="inlineStr"/>
@@ -12038,12 +11974,12 @@
       <c r="U152" t="inlineStr"/>
       <c r="V152" t="inlineStr">
         <is>
-          <t>MsAcPdmpDt</t>
+          <t>AnyPdmpFr</t>
         </is>
       </c>
       <c r="W152" t="inlineStr">
         <is>
-          <t>Must-Access PDMP start date</t>
+          <t>Any PDMP (fraction of year in 2017)</t>
         </is>
       </c>
       <c r="X152" t="inlineStr"/>
@@ -12126,12 +12062,12 @@
       <c r="U153" t="inlineStr"/>
       <c r="V153" t="inlineStr">
         <is>
-          <t>MsAcPdmpFr</t>
+          <t>AnyPdmphDt</t>
         </is>
       </c>
       <c r="W153" t="inlineStr">
         <is>
-          <t>Must-Access PDMP (fraction of year in 2017)</t>
+          <t>Any Horowitz PDMP start date</t>
         </is>
       </c>
       <c r="X153" t="inlineStr"/>
@@ -12214,12 +12150,12 @@
       <c r="U154" t="inlineStr"/>
       <c r="V154" t="inlineStr">
         <is>
-          <t>OpPdmpDt</t>
+          <t>AnyPdmphFr</t>
         </is>
       </c>
       <c r="W154" t="inlineStr">
         <is>
-          <t>Operational PDMP start date</t>
+          <t>Any Horowitz PDMP (fraction of year in 2017)</t>
         </is>
       </c>
       <c r="X154" t="inlineStr"/>
@@ -12302,12 +12238,12 @@
       <c r="U155" t="inlineStr"/>
       <c r="V155" t="inlineStr">
         <is>
-          <t>OpPdmpFr</t>
+          <t>ElcPdmpDt</t>
         </is>
       </c>
       <c r="W155" t="inlineStr">
         <is>
-          <t>Operational PDMP (fraction of year in 2017)</t>
+          <t>Electronic PDMP start date</t>
         </is>
       </c>
       <c r="X155" t="inlineStr"/>
@@ -12338,7 +12274,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>State &amp; Local Government Expenditures</t>
+          <t>Prescription Drug Monitoring Programs (PDMP)</t>
         </is>
       </c>
       <c r="C156" t="inlineStr"/>
@@ -12349,8 +12285,16 @@
       <c r="H156" t="inlineStr"/>
       <c r="I156" t="inlineStr"/>
       <c r="J156" t="inlineStr"/>
-      <c r="K156" t="inlineStr"/>
-      <c r="L156" t="inlineStr"/>
+      <c r="K156" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="L156" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="M156" t="inlineStr">
         <is>
           <t>x</t>
@@ -12371,35 +12315,39 @@
           <t>x</t>
         </is>
       </c>
-      <c r="Q156" t="inlineStr"/>
+      <c r="Q156" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="R156" t="inlineStr"/>
       <c r="S156" t="inlineStr"/>
       <c r="T156" t="inlineStr"/>
       <c r="U156" t="inlineStr"/>
       <c r="V156" t="inlineStr">
         <is>
-          <t>CrrctExp</t>
+          <t>ElcPdmpFr</t>
         </is>
       </c>
       <c r="W156" t="inlineStr">
         <is>
-          <t>Corrections expenditures</t>
+          <t>Electronic PDMP (fraction of year in 2017)</t>
         </is>
       </c>
       <c r="X156" t="inlineStr"/>
       <c r="Y156" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Public_Expenditures.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/PDMP_Presence.md</t>
         </is>
       </c>
       <c r="Z156" t="inlineStr">
         <is>
-          <t>Survey of State and Local Government Finances 2018-2022</t>
+          <t>OPTIC 2017-2022</t>
         </is>
       </c>
       <c r="AA156" t="inlineStr">
         <is>
-          <t>U.S. Census Bureau Annual Survey of State and Local Government Finances via Urban Institute &amp; Tax Policy Center's State and Local Finance Data Finder</t>
+          <t>RAND-USC Schaeffer Opioid Policy Tools and Information Center, 2017-2022</t>
         </is>
       </c>
       <c r="AB156" t="inlineStr"/>
@@ -12414,7 +12362,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>State &amp; Local Government Expenditures</t>
+          <t>Prescription Drug Monitoring Programs (PDMP)</t>
         </is>
       </c>
       <c r="C157" t="inlineStr"/>
@@ -12425,16 +12373,36 @@
       <c r="H157" t="inlineStr"/>
       <c r="I157" t="inlineStr"/>
       <c r="J157" t="inlineStr"/>
-      <c r="K157" t="inlineStr"/>
+      <c r="K157" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L157" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="M157" t="inlineStr"/>
-      <c r="N157" t="inlineStr"/>
-      <c r="O157" t="inlineStr"/>
-      <c r="P157" t="inlineStr"/>
+      <c r="M157" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="N157" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="O157" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="P157" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q157" t="inlineStr">
         <is>
           <t>x</t>
@@ -12446,28 +12414,28 @@
       <c r="U157" t="inlineStr"/>
       <c r="V157" t="inlineStr">
         <is>
-          <t>ExpnFedExp</t>
+          <t>MsAcPdmpDt</t>
         </is>
       </c>
       <c r="W157" t="inlineStr">
         <is>
-          <t>Expansion Medicaid Federal Spending</t>
+          <t>Must-Access PDMP start date</t>
         </is>
       </c>
       <c r="X157" t="inlineStr"/>
       <c r="Y157" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Medical_Expenditures.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/PDMP_Presence.md</t>
         </is>
       </c>
       <c r="Z157" t="inlineStr">
         <is>
-          <t>KFF 2018, 2019</t>
+          <t>OPTIC 2017-2022</t>
         </is>
       </c>
       <c r="AA157" t="inlineStr">
         <is>
-          <t>Kaiser Family Foundation,  2018, 2019</t>
+          <t>RAND-USC Schaeffer Opioid Policy Tools and Information Center, 2017-2022</t>
         </is>
       </c>
       <c r="AB157" t="inlineStr"/>
@@ -12482,7 +12450,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>State &amp; Local Government Expenditures</t>
+          <t>Prescription Drug Monitoring Programs (PDMP)</t>
         </is>
       </c>
       <c r="C158" t="inlineStr"/>
@@ -12493,16 +12461,36 @@
       <c r="H158" t="inlineStr"/>
       <c r="I158" t="inlineStr"/>
       <c r="J158" t="inlineStr"/>
-      <c r="K158" t="inlineStr"/>
+      <c r="K158" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L158" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="M158" t="inlineStr"/>
-      <c r="N158" t="inlineStr"/>
-      <c r="O158" t="inlineStr"/>
-      <c r="P158" t="inlineStr"/>
+      <c r="M158" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="N158" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="O158" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="P158" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q158" t="inlineStr">
         <is>
           <t>x</t>
@@ -12514,28 +12502,28 @@
       <c r="U158" t="inlineStr"/>
       <c r="V158" t="inlineStr">
         <is>
-          <t>ExpnSttExp</t>
+          <t>MsAcPdmpFr</t>
         </is>
       </c>
       <c r="W158" t="inlineStr">
         <is>
-          <t>Expansion Medicaid State Spending</t>
+          <t>Must-Access PDMP (fraction of year in 2017)</t>
         </is>
       </c>
       <c r="X158" t="inlineStr"/>
       <c r="Y158" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Medical_Expenditures.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/PDMP_Presence.md</t>
         </is>
       </c>
       <c r="Z158" t="inlineStr">
         <is>
-          <t>KFF 2018, 2019</t>
+          <t>OPTIC 2017-2022</t>
         </is>
       </c>
       <c r="AA158" t="inlineStr">
         <is>
-          <t>Kaiser Family Foundation,  2018, 2019</t>
+          <t>RAND-USC Schaeffer Opioid Policy Tools and Information Center, 2017-2022</t>
         </is>
       </c>
       <c r="AB158" t="inlineStr"/>
@@ -12550,7 +12538,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>State &amp; Local Government Expenditures</t>
+          <t>Prescription Drug Monitoring Programs (PDMP)</t>
         </is>
       </c>
       <c r="C159" t="inlineStr"/>
@@ -12561,8 +12549,16 @@
       <c r="H159" t="inlineStr"/>
       <c r="I159" t="inlineStr"/>
       <c r="J159" t="inlineStr"/>
-      <c r="K159" t="inlineStr"/>
-      <c r="L159" t="inlineStr"/>
+      <c r="K159" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="L159" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="M159" t="inlineStr">
         <is>
           <t>x</t>
@@ -12583,35 +12579,39 @@
           <t>x</t>
         </is>
       </c>
-      <c r="Q159" t="inlineStr"/>
+      <c r="Q159" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="R159" t="inlineStr"/>
       <c r="S159" t="inlineStr"/>
       <c r="T159" t="inlineStr"/>
       <c r="U159" t="inlineStr"/>
       <c r="V159" t="inlineStr">
         <is>
-          <t>HlthExp</t>
+          <t>OpPdmpDt</t>
         </is>
       </c>
       <c r="W159" t="inlineStr">
         <is>
-          <t>Public health expenditures</t>
+          <t>Operational PDMP start date</t>
         </is>
       </c>
       <c r="X159" t="inlineStr"/>
       <c r="Y159" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Public_Expenditures.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/PDMP_Presence.md</t>
         </is>
       </c>
       <c r="Z159" t="inlineStr">
         <is>
-          <t>Survey of State and Local Government Finances 2018-2022</t>
+          <t>OPTIC 2017-2022</t>
         </is>
       </c>
       <c r="AA159" t="inlineStr">
         <is>
-          <t>U.S. Census Bureau Annual Survey of State and Local Government Finances via Urban Institute &amp; Tax Policy Center's State and Local Finance Data Finder</t>
+          <t>RAND-USC Schaeffer Opioid Policy Tools and Information Center, 2017-2022</t>
         </is>
       </c>
       <c r="AB159" t="inlineStr"/>
@@ -12626,7 +12626,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>State &amp; Local Government Expenditures</t>
+          <t>Prescription Drug Monitoring Programs (PDMP)</t>
         </is>
       </c>
       <c r="C160" t="inlineStr"/>
@@ -12637,7 +12637,11 @@
       <c r="H160" t="inlineStr"/>
       <c r="I160" t="inlineStr"/>
       <c r="J160" t="inlineStr"/>
-      <c r="K160" t="inlineStr"/>
+      <c r="K160" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L160" t="inlineStr">
         <is>
           <t>x</t>
@@ -12648,9 +12652,21 @@
           <t>x</t>
         </is>
       </c>
-      <c r="N160" t="inlineStr"/>
-      <c r="O160" t="inlineStr"/>
-      <c r="P160" t="inlineStr"/>
+      <c r="N160" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="O160" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="P160" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q160" t="inlineStr">
         <is>
           <t>x</t>
@@ -12662,28 +12678,28 @@
       <c r="U160" t="inlineStr"/>
       <c r="V160" t="inlineStr">
         <is>
-          <t>MedcdExp</t>
+          <t>OpPdmpFr</t>
         </is>
       </c>
       <c r="W160" t="inlineStr">
         <is>
-          <t>Total Medicaid Spending</t>
+          <t>Operational PDMP (fraction of year in 2017)</t>
         </is>
       </c>
       <c r="X160" t="inlineStr"/>
       <c r="Y160" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Medical_Expenditures.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/PDMP_Presence.md</t>
         </is>
       </c>
       <c r="Z160" t="inlineStr">
         <is>
-          <t>KFF 2018, 2019</t>
+          <t>OPTIC 2017-2022</t>
         </is>
       </c>
       <c r="AA160" t="inlineStr">
         <is>
-          <t>Kaiser Family Foundation,  2018, 2019</t>
+          <t>RAND-USC Schaeffer Opioid Policy Tools and Information Center, 2017-2022</t>
         </is>
       </c>
       <c r="AB160" t="inlineStr"/>
@@ -12738,12 +12754,12 @@
       <c r="U161" t="inlineStr"/>
       <c r="V161" t="inlineStr">
         <is>
-          <t>PlcFyrExp</t>
+          <t>CrrctExp</t>
         </is>
       </c>
       <c r="W161" t="inlineStr">
         <is>
-          <t>Police &amp; fire expenditures</t>
+          <t>Corrections expenditures</t>
         </is>
       </c>
       <c r="X161" t="inlineStr"/>
@@ -12806,12 +12822,12 @@
       <c r="U162" t="inlineStr"/>
       <c r="V162" t="inlineStr">
         <is>
-          <t>TradFedExp</t>
+          <t>ExpnFedExp</t>
         </is>
       </c>
       <c r="W162" t="inlineStr">
         <is>
-          <t>Traditional Medicaid Federal Spending</t>
+          <t>Expansion Medicaid Federal Spending</t>
         </is>
       </c>
       <c r="X162" t="inlineStr"/>
@@ -12874,12 +12890,12 @@
       <c r="U163" t="inlineStr"/>
       <c r="V163" t="inlineStr">
         <is>
-          <t>TradSttExp</t>
+          <t>ExpnSttExp</t>
         </is>
       </c>
       <c r="W163" t="inlineStr">
         <is>
-          <t>Traditional Medicaid State Spending</t>
+          <t>Expansion Medicaid State Spending</t>
         </is>
       </c>
       <c r="X163" t="inlineStr"/>
@@ -12950,12 +12966,12 @@
       <c r="U164" t="inlineStr"/>
       <c r="V164" t="inlineStr">
         <is>
-          <t>WlfrExp</t>
+          <t>HlthExp</t>
         </is>
       </c>
       <c r="W164" t="inlineStr">
         <is>
-          <t>Public welfare expenditures</t>
+          <t>Public health expenditures</t>
         </is>
       </c>
       <c r="X164" t="inlineStr"/>
@@ -12981,12 +12997,12 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>Outcome</t>
+          <t>Policy</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Hepatitis C Rates</t>
+          <t>State &amp; Local Government Expenditures</t>
         </is>
       </c>
       <c r="C165" t="inlineStr"/>
@@ -12997,45 +13013,53 @@
       <c r="H165" t="inlineStr"/>
       <c r="I165" t="inlineStr"/>
       <c r="J165" t="inlineStr"/>
-      <c r="K165" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="L165" t="inlineStr"/>
-      <c r="M165" t="inlineStr"/>
+      <c r="K165" t="inlineStr"/>
+      <c r="L165" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="M165" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="N165" t="inlineStr"/>
       <c r="O165" t="inlineStr"/>
       <c r="P165" t="inlineStr"/>
-      <c r="Q165" t="inlineStr"/>
+      <c r="Q165" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="R165" t="inlineStr"/>
       <c r="S165" t="inlineStr"/>
       <c r="T165" t="inlineStr"/>
       <c r="U165" t="inlineStr"/>
       <c r="V165" t="inlineStr">
         <is>
-          <t>A50_74Hcv</t>
+          <t>MedcdExp</t>
         </is>
       </c>
       <c r="W165" t="inlineStr">
         <is>
-          <t>Yearly Hepatitis C cases - 50 to 74 years old (2013-2016)</t>
+          <t>Total Medicaid Spending</t>
         </is>
       </c>
       <c r="X165" t="inlineStr"/>
       <c r="Y165" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/HepatitisC_Rates.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Medical_Expenditures.md</t>
         </is>
       </c>
       <c r="Z165" t="inlineStr">
         <is>
-          <t>HepVu 2013-2016, 2018-2022</t>
+          <t>KFF 2018, 2019</t>
         </is>
       </c>
       <c r="AA165" t="inlineStr">
         <is>
-          <t>HepVu, Emory University Rollins School of Public Health, 2013-2016 &amp; 2018-2022</t>
+          <t>Kaiser Family Foundation,  2018, 2019</t>
         </is>
       </c>
       <c r="AB165" t="inlineStr"/>
@@ -13045,48 +13069,24 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>Outcome</t>
+          <t>Policy</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Hepatitis C Rates</t>
+          <t>State &amp; Local Government Expenditures</t>
         </is>
       </c>
       <c r="C166" t="inlineStr"/>
       <c r="D166" t="inlineStr"/>
       <c r="E166" t="inlineStr"/>
       <c r="F166" t="inlineStr"/>
-      <c r="G166" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="H166" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="I166" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="J166" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="K166" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="L166" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="G166" t="inlineStr"/>
+      <c r="H166" t="inlineStr"/>
+      <c r="I166" t="inlineStr"/>
+      <c r="J166" t="inlineStr"/>
+      <c r="K166" t="inlineStr"/>
+      <c r="L166" t="inlineStr"/>
       <c r="M166" t="inlineStr">
         <is>
           <t>x</t>
@@ -13114,28 +13114,28 @@
       <c r="U166" t="inlineStr"/>
       <c r="V166" t="inlineStr">
         <is>
-          <t>A50_74HcvD</t>
+          <t>PlcFyrExp</t>
         </is>
       </c>
       <c r="W166" t="inlineStr">
         <is>
-          <t>Hepatitis C Deaths - 50 to 74 years old</t>
+          <t>Police &amp; fire expenditures</t>
         </is>
       </c>
       <c r="X166" t="inlineStr"/>
       <c r="Y166" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/HepatitisC_Rates.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Public_Expenditures.md</t>
         </is>
       </c>
       <c r="Z166" t="inlineStr">
         <is>
-          <t>HepVu 2013-2016, 2018-2022</t>
+          <t>Survey of State and Local Government Finances 2018-2022</t>
         </is>
       </c>
       <c r="AA166" t="inlineStr">
         <is>
-          <t>HepVu, Emory University Rollins School of Public Health, 2013-2016 &amp; 2018-2022</t>
+          <t>U.S. Census Bureau Annual Survey of State and Local Government Finances via Urban Institute &amp; Tax Policy Center's State and Local Finance Data Finder</t>
         </is>
       </c>
       <c r="AB166" t="inlineStr"/>
@@ -13145,97 +13145,65 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>Outcome</t>
+          <t>Policy</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Hepatitis C Rates</t>
+          <t>State &amp; Local Government Expenditures</t>
         </is>
       </c>
       <c r="C167" t="inlineStr"/>
       <c r="D167" t="inlineStr"/>
       <c r="E167" t="inlineStr"/>
       <c r="F167" t="inlineStr"/>
-      <c r="G167" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="H167" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="I167" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="J167" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="K167" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="G167" t="inlineStr"/>
+      <c r="H167" t="inlineStr"/>
+      <c r="I167" t="inlineStr"/>
+      <c r="J167" t="inlineStr"/>
+      <c r="K167" t="inlineStr"/>
       <c r="L167" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="M167" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="N167" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="O167" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="P167" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="Q167" t="inlineStr"/>
+      <c r="M167" t="inlineStr"/>
+      <c r="N167" t="inlineStr"/>
+      <c r="O167" t="inlineStr"/>
+      <c r="P167" t="inlineStr"/>
+      <c r="Q167" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="R167" t="inlineStr"/>
       <c r="S167" t="inlineStr"/>
       <c r="T167" t="inlineStr"/>
       <c r="U167" t="inlineStr"/>
       <c r="V167" t="inlineStr">
         <is>
-          <t>AmInHcvD</t>
+          <t>TradFedExp</t>
         </is>
       </c>
       <c r="W167" t="inlineStr">
         <is>
-          <t>Hepatitis C Deaths - American Indian</t>
+          <t>Traditional Medicaid Federal Spending</t>
         </is>
       </c>
       <c r="X167" t="inlineStr"/>
       <c r="Y167" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/HepatitisC_Rates.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Medical_Expenditures.md</t>
         </is>
       </c>
       <c r="Z167" t="inlineStr">
         <is>
-          <t>HepVu 2013-2016, 2018-2022</t>
+          <t>KFF 2018, 2019</t>
         </is>
       </c>
       <c r="AA167" t="inlineStr">
         <is>
-          <t>HepVu, Emory University Rollins School of Public Health, 2013-2016 &amp; 2018-2022</t>
+          <t>Kaiser Family Foundation,  2018, 2019</t>
         </is>
       </c>
       <c r="AB167" t="inlineStr"/>
@@ -13245,12 +13213,12 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Outcome</t>
+          <t>Policy</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Hepatitis C Rates</t>
+          <t>State &amp; Local Government Expenditures</t>
         </is>
       </c>
       <c r="C168" t="inlineStr"/>
@@ -13267,55 +13235,43 @@
           <t>x</t>
         </is>
       </c>
-      <c r="M168" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="N168" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="O168" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="P168" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="Q168" t="inlineStr"/>
+      <c r="M168" t="inlineStr"/>
+      <c r="N168" t="inlineStr"/>
+      <c r="O168" t="inlineStr"/>
+      <c r="P168" t="inlineStr"/>
+      <c r="Q168" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="R168" t="inlineStr"/>
       <c r="S168" t="inlineStr"/>
       <c r="T168" t="inlineStr"/>
       <c r="U168" t="inlineStr"/>
       <c r="V168" t="inlineStr">
         <is>
-          <t>AsHcvD</t>
+          <t>TradSttExp</t>
         </is>
       </c>
       <c r="W168" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hepatitis C deaths among Asian populations </t>
+          <t>Traditional Medicaid State Spending</t>
         </is>
       </c>
       <c r="X168" t="inlineStr"/>
       <c r="Y168" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/HepatitisC_Rates.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Medical_Expenditures.md</t>
         </is>
       </c>
       <c r="Z168" t="inlineStr">
         <is>
-          <t>HepVu 2013-2016, 2018-2022</t>
+          <t>KFF 2018, 2019</t>
         </is>
       </c>
       <c r="AA168" t="inlineStr">
         <is>
-          <t>HepVu, Emory University Rollins School of Public Health, 2013-2016 &amp; 2018-2022</t>
+          <t>Kaiser Family Foundation,  2018, 2019</t>
         </is>
       </c>
       <c r="AB168" t="inlineStr"/>
@@ -13325,48 +13281,44 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Outcome</t>
+          <t>Policy</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Hepatitis C Rates</t>
+          <t>State &amp; Local Government Expenditures</t>
         </is>
       </c>
       <c r="C169" t="inlineStr"/>
       <c r="D169" t="inlineStr"/>
       <c r="E169" t="inlineStr"/>
       <c r="F169" t="inlineStr"/>
-      <c r="G169" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="H169" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="I169" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="J169" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="K169" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="G169" t="inlineStr"/>
+      <c r="H169" t="inlineStr"/>
+      <c r="I169" t="inlineStr"/>
+      <c r="J169" t="inlineStr"/>
+      <c r="K169" t="inlineStr"/>
       <c r="L169" t="inlineStr"/>
-      <c r="M169" t="inlineStr"/>
-      <c r="N169" t="inlineStr"/>
-      <c r="O169" t="inlineStr"/>
-      <c r="P169" t="inlineStr"/>
+      <c r="M169" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="N169" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="O169" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="P169" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q169" t="inlineStr"/>
       <c r="R169" t="inlineStr"/>
       <c r="S169" t="inlineStr"/>
@@ -13374,28 +13326,28 @@
       <c r="U169" t="inlineStr"/>
       <c r="V169" t="inlineStr">
         <is>
-          <t>AsPiHcvD</t>
+          <t>WlfrExp</t>
         </is>
       </c>
       <c r="W169" t="inlineStr">
         <is>
-          <t>Hepatitis C Deaths - Asian &amp; Pacific Islander</t>
+          <t>Public welfare expenditures</t>
         </is>
       </c>
       <c r="X169" t="inlineStr"/>
       <c r="Y169" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/HepatitisC_Rates.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Public_Expenditures.md</t>
         </is>
       </c>
       <c r="Z169" t="inlineStr">
         <is>
-          <t>HepVu 2013-2016, 2018-2022</t>
+          <t>Survey of State and Local Government Finances 2018-2022</t>
         </is>
       </c>
       <c r="AA169" t="inlineStr">
         <is>
-          <t>HepVu, Emory University Rollins School of Public Health, 2013-2016 &amp; 2018-2022</t>
+          <t>U.S. Census Bureau Annual Survey of State and Local Government Finances via Urban Institute &amp; Tax Policy Center's State and Local Finance Data Finder</t>
         </is>
       </c>
       <c r="AB169" t="inlineStr"/>
@@ -13430,11 +13382,7 @@
       <c r="M170" t="inlineStr"/>
       <c r="N170" t="inlineStr"/>
       <c r="O170" t="inlineStr"/>
-      <c r="P170" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P170" t="inlineStr"/>
       <c r="Q170" t="inlineStr"/>
       <c r="R170" t="inlineStr"/>
       <c r="S170" t="inlineStr"/>
@@ -13442,12 +13390,12 @@
       <c r="U170" t="inlineStr"/>
       <c r="V170" t="inlineStr">
         <is>
-          <t>AvA50_74HcvD</t>
+          <t>A50_74Hcv</t>
         </is>
       </c>
       <c r="W170" t="inlineStr">
         <is>
-          <t>Average Ages between 50 to 74 Hepitatis C virus Deaths</t>
+          <t>Yearly Hepatitis C cases - 50 to 74 years old (2013-2016)</t>
         </is>
       </c>
       <c r="X170" t="inlineStr"/>
@@ -13485,19 +13433,51 @@
       <c r="D171" t="inlineStr"/>
       <c r="E171" t="inlineStr"/>
       <c r="F171" t="inlineStr"/>
-      <c r="G171" t="inlineStr"/>
-      <c r="H171" t="inlineStr"/>
-      <c r="I171" t="inlineStr"/>
-      <c r="J171" t="inlineStr"/>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H171" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="I171" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="J171" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="K171" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="L171" t="inlineStr"/>
-      <c r="M171" t="inlineStr"/>
-      <c r="N171" t="inlineStr"/>
-      <c r="O171" t="inlineStr"/>
+      <c r="L171" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="M171" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="N171" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="O171" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="P171" t="inlineStr">
         <is>
           <t>x</t>
@@ -13510,12 +13490,12 @@
       <c r="U171" t="inlineStr"/>
       <c r="V171" t="inlineStr">
         <is>
-          <t>AvAmInHcvD</t>
+          <t>A50_74HcvD</t>
         </is>
       </c>
       <c r="W171" t="inlineStr">
         <is>
-          <t>Hepatitis C Deaths - American Indian (5-Year Averages)</t>
+          <t>Hepatitis C Deaths - 50 to 74 years old</t>
         </is>
       </c>
       <c r="X171" t="inlineStr"/>
@@ -13553,15 +13533,51 @@
       <c r="D172" t="inlineStr"/>
       <c r="E172" t="inlineStr"/>
       <c r="F172" t="inlineStr"/>
-      <c r="G172" t="inlineStr"/>
-      <c r="H172" t="inlineStr"/>
-      <c r="I172" t="inlineStr"/>
-      <c r="J172" t="inlineStr"/>
-      <c r="K172" t="inlineStr"/>
-      <c r="L172" t="inlineStr"/>
-      <c r="M172" t="inlineStr"/>
-      <c r="N172" t="inlineStr"/>
-      <c r="O172" t="inlineStr"/>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H172" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="I172" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="J172" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="K172" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="L172" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="M172" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="N172" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="O172" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="P172" t="inlineStr">
         <is>
           <t>x</t>
@@ -13574,12 +13590,12 @@
       <c r="U172" t="inlineStr"/>
       <c r="V172" t="inlineStr">
         <is>
-          <t>AvAsHcvD</t>
+          <t>AmInHcvD</t>
         </is>
       </c>
       <c r="W172" t="inlineStr">
         <is>
-          <t>Mean yearly Hepatitis C deaths among Asian population from 2018-2022</t>
+          <t>Hepatitis C Deaths - American Indian</t>
         </is>
       </c>
       <c r="X172" t="inlineStr"/>
@@ -13621,16 +13637,32 @@
       <c r="H173" t="inlineStr"/>
       <c r="I173" t="inlineStr"/>
       <c r="J173" t="inlineStr"/>
-      <c r="K173" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="L173" t="inlineStr"/>
-      <c r="M173" t="inlineStr"/>
-      <c r="N173" t="inlineStr"/>
-      <c r="O173" t="inlineStr"/>
-      <c r="P173" t="inlineStr"/>
+      <c r="K173" t="inlineStr"/>
+      <c r="L173" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="M173" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="N173" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="O173" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="P173" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q173" t="inlineStr"/>
       <c r="R173" t="inlineStr"/>
       <c r="S173" t="inlineStr"/>
@@ -13638,12 +13670,12 @@
       <c r="U173" t="inlineStr"/>
       <c r="V173" t="inlineStr">
         <is>
-          <t>AvAsPiHcvD</t>
+          <t>AsHcvD</t>
         </is>
       </c>
       <c r="W173" t="inlineStr">
         <is>
-          <t>Hepatitis C Deaths - Asian &amp; Pacific Islander (2013 - 2017)</t>
+          <t xml:space="preserve">Hepatitis C deaths among Asian populations </t>
         </is>
       </c>
       <c r="X173" t="inlineStr"/>
@@ -13681,10 +13713,26 @@
       <c r="D174" t="inlineStr"/>
       <c r="E174" t="inlineStr"/>
       <c r="F174" t="inlineStr"/>
-      <c r="G174" t="inlineStr"/>
-      <c r="H174" t="inlineStr"/>
-      <c r="I174" t="inlineStr"/>
-      <c r="J174" t="inlineStr"/>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H174" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="I174" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="J174" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="K174" t="inlineStr">
         <is>
           <t>x</t>
@@ -13694,11 +13742,7 @@
       <c r="M174" t="inlineStr"/>
       <c r="N174" t="inlineStr"/>
       <c r="O174" t="inlineStr"/>
-      <c r="P174" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P174" t="inlineStr"/>
       <c r="Q174" t="inlineStr"/>
       <c r="R174" t="inlineStr"/>
       <c r="S174" t="inlineStr"/>
@@ -13706,12 +13750,12 @@
       <c r="U174" t="inlineStr"/>
       <c r="V174" t="inlineStr">
         <is>
-          <t>AvBlkHcvD</t>
+          <t>AsPiHcvD</t>
         </is>
       </c>
       <c r="W174" t="inlineStr">
         <is>
-          <t>Hepatitis C Deaths - Black (5-Year Averages)</t>
+          <t>Hepatitis C Deaths - Asian &amp; Pacific Islander</t>
         </is>
       </c>
       <c r="X174" t="inlineStr"/>
@@ -13774,12 +13818,12 @@
       <c r="U175" t="inlineStr"/>
       <c r="V175" t="inlineStr">
         <is>
-          <t>AvFlHcvD</t>
+          <t>AvA50_74HcvD</t>
         </is>
       </c>
       <c r="W175" t="inlineStr">
         <is>
-          <t>Hepatitis C Deaths - Women (5-Year Averages)</t>
+          <t>Average Ages between 50 to 74 Hepitatis C virus Deaths</t>
         </is>
       </c>
       <c r="X175" t="inlineStr"/>
@@ -13842,12 +13886,12 @@
       <c r="U176" t="inlineStr"/>
       <c r="V176" t="inlineStr">
         <is>
-          <t>AvHcvD</t>
+          <t>AvAmInHcvD</t>
         </is>
       </c>
       <c r="W176" t="inlineStr">
         <is>
-          <t>Average Hepitatis C virus Deaths (5-Year Averages)</t>
+          <t>Hepatitis C Deaths - American Indian (5-Year Averages)</t>
         </is>
       </c>
       <c r="X176" t="inlineStr"/>
@@ -13889,11 +13933,7 @@
       <c r="H177" t="inlineStr"/>
       <c r="I177" t="inlineStr"/>
       <c r="J177" t="inlineStr"/>
-      <c r="K177" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K177" t="inlineStr"/>
       <c r="L177" t="inlineStr"/>
       <c r="M177" t="inlineStr"/>
       <c r="N177" t="inlineStr"/>
@@ -13910,12 +13950,12 @@
       <c r="U177" t="inlineStr"/>
       <c r="V177" t="inlineStr">
         <is>
-          <t>AvHspHcvD</t>
+          <t>AvAsHcvD</t>
         </is>
       </c>
       <c r="W177" t="inlineStr">
         <is>
-          <t>Hepatitis C Deaths - Hispanic (5-Year Averages)</t>
+          <t>Mean yearly Hepatitis C deaths among Asian population from 2018-2022</t>
         </is>
       </c>
       <c r="X177" t="inlineStr"/>
@@ -13966,11 +14006,7 @@
       <c r="M178" t="inlineStr"/>
       <c r="N178" t="inlineStr"/>
       <c r="O178" t="inlineStr"/>
-      <c r="P178" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P178" t="inlineStr"/>
       <c r="Q178" t="inlineStr"/>
       <c r="R178" t="inlineStr"/>
       <c r="S178" t="inlineStr"/>
@@ -13978,12 +14014,12 @@
       <c r="U178" t="inlineStr"/>
       <c r="V178" t="inlineStr">
         <is>
-          <t>AvMlHcvD</t>
+          <t>AvAsPiHcvD</t>
         </is>
       </c>
       <c r="W178" t="inlineStr">
         <is>
-          <t>Hepatitis C Deaths - Men (5-Year Averages)</t>
+          <t>Hepatitis C Deaths - Asian &amp; Pacific Islander (2013 - 2017)</t>
         </is>
       </c>
       <c r="X178" t="inlineStr"/>
@@ -14025,7 +14061,11 @@
       <c r="H179" t="inlineStr"/>
       <c r="I179" t="inlineStr"/>
       <c r="J179" t="inlineStr"/>
-      <c r="K179" t="inlineStr"/>
+      <c r="K179" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L179" t="inlineStr"/>
       <c r="M179" t="inlineStr"/>
       <c r="N179" t="inlineStr"/>
@@ -14042,12 +14082,12 @@
       <c r="U179" t="inlineStr"/>
       <c r="V179" t="inlineStr">
         <is>
-          <t>AvMulHcvD</t>
+          <t>AvBlkHcvD</t>
         </is>
       </c>
       <c r="W179" t="inlineStr">
         <is>
-          <t>Mean yearly Hepatitis C deaths among Multiple Race populations from 2018-2022</t>
+          <t>Hepatitis C Deaths - Black (5-Year Averages)</t>
         </is>
       </c>
       <c r="X179" t="inlineStr"/>
@@ -14089,7 +14129,11 @@
       <c r="H180" t="inlineStr"/>
       <c r="I180" t="inlineStr"/>
       <c r="J180" t="inlineStr"/>
-      <c r="K180" t="inlineStr"/>
+      <c r="K180" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L180" t="inlineStr"/>
       <c r="M180" t="inlineStr"/>
       <c r="N180" t="inlineStr"/>
@@ -14106,12 +14150,12 @@
       <c r="U180" t="inlineStr"/>
       <c r="V180" t="inlineStr">
         <is>
-          <t>AvNhPiHcvD</t>
+          <t>AvFlHcvD</t>
         </is>
       </c>
       <c r="W180" t="inlineStr">
         <is>
-          <t>Mean yearly Hepatitis C deaths among Native Hawaiian and Pacific Islanders population from 2018-2022</t>
+          <t>Hepatitis C Deaths - Women (5-Year Averages)</t>
         </is>
       </c>
       <c r="X180" t="inlineStr"/>
@@ -14174,12 +14218,12 @@
       <c r="U181" t="inlineStr"/>
       <c r="V181" t="inlineStr">
         <is>
-          <t>AvO75HcvD</t>
+          <t>AvHcvD</t>
         </is>
       </c>
       <c r="W181" t="inlineStr">
         <is>
-          <t>Hepatitis C Deaths - Age Over 75  (5-Year Averages)</t>
+          <t>Average Hepitatis C virus Deaths (5-Year Averages)</t>
         </is>
       </c>
       <c r="X181" t="inlineStr"/>
@@ -14242,12 +14286,12 @@
       <c r="U182" t="inlineStr"/>
       <c r="V182" t="inlineStr">
         <is>
-          <t>AvU50HcvD</t>
+          <t>AvHspHcvD</t>
         </is>
       </c>
       <c r="W182" t="inlineStr">
         <is>
-          <t>Hepatitis C Deaths - Age Under 50 (5-Year Averages)</t>
+          <t>Hepatitis C Deaths - Hispanic (5-Year Averages)</t>
         </is>
       </c>
       <c r="X182" t="inlineStr"/>
@@ -14289,7 +14333,11 @@
       <c r="H183" t="inlineStr"/>
       <c r="I183" t="inlineStr"/>
       <c r="J183" t="inlineStr"/>
-      <c r="K183" t="inlineStr"/>
+      <c r="K183" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L183" t="inlineStr"/>
       <c r="M183" t="inlineStr"/>
       <c r="N183" t="inlineStr"/>
@@ -14306,12 +14354,12 @@
       <c r="U183" t="inlineStr"/>
       <c r="V183" t="inlineStr">
         <is>
-          <t>AvWhHcvD</t>
+          <t>AvMlHcvD</t>
         </is>
       </c>
       <c r="W183" t="inlineStr">
         <is>
-          <t>Average White Hepitatis C virus Deaths</t>
+          <t>Hepatitis C Deaths - Men (5-Year Averages)</t>
         </is>
       </c>
       <c r="X183" t="inlineStr"/>
@@ -14353,16 +14401,16 @@
       <c r="H184" t="inlineStr"/>
       <c r="I184" t="inlineStr"/>
       <c r="J184" t="inlineStr"/>
-      <c r="K184" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K184" t="inlineStr"/>
       <c r="L184" t="inlineStr"/>
       <c r="M184" t="inlineStr"/>
       <c r="N184" t="inlineStr"/>
       <c r="O184" t="inlineStr"/>
-      <c r="P184" t="inlineStr"/>
+      <c r="P184" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q184" t="inlineStr"/>
       <c r="R184" t="inlineStr"/>
       <c r="S184" t="inlineStr"/>
@@ -14370,12 +14418,12 @@
       <c r="U184" t="inlineStr"/>
       <c r="V184" t="inlineStr">
         <is>
-          <t>BlkHcv</t>
+          <t>AvMulHcvD</t>
         </is>
       </c>
       <c r="W184" t="inlineStr">
         <is>
-          <t>Yearly Hepatitis C cases - Black (2013-2016)</t>
+          <t>Mean yearly Hepatitis C deaths among Multiple Race populations from 2018-2022</t>
         </is>
       </c>
       <c r="X184" t="inlineStr"/>
@@ -14413,51 +14461,15 @@
       <c r="D185" t="inlineStr"/>
       <c r="E185" t="inlineStr"/>
       <c r="F185" t="inlineStr"/>
-      <c r="G185" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="H185" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="I185" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="J185" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="K185" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="L185" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="M185" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="N185" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="O185" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="G185" t="inlineStr"/>
+      <c r="H185" t="inlineStr"/>
+      <c r="I185" t="inlineStr"/>
+      <c r="J185" t="inlineStr"/>
+      <c r="K185" t="inlineStr"/>
+      <c r="L185" t="inlineStr"/>
+      <c r="M185" t="inlineStr"/>
+      <c r="N185" t="inlineStr"/>
+      <c r="O185" t="inlineStr"/>
       <c r="P185" t="inlineStr">
         <is>
           <t>x</t>
@@ -14470,12 +14482,12 @@
       <c r="U185" t="inlineStr"/>
       <c r="V185" t="inlineStr">
         <is>
-          <t>BlkHcvD</t>
+          <t>AvNhPiHcvD</t>
         </is>
       </c>
       <c r="W185" t="inlineStr">
         <is>
-          <t>Hepatitis C Deaths - Black</t>
+          <t>Mean yearly Hepatitis C deaths among Native Hawaiian and Pacific Islanders population from 2018-2022</t>
         </is>
       </c>
       <c r="X185" t="inlineStr"/>
@@ -14513,51 +14525,19 @@
       <c r="D186" t="inlineStr"/>
       <c r="E186" t="inlineStr"/>
       <c r="F186" t="inlineStr"/>
-      <c r="G186" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="H186" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="I186" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="J186" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="G186" t="inlineStr"/>
+      <c r="H186" t="inlineStr"/>
+      <c r="I186" t="inlineStr"/>
+      <c r="J186" t="inlineStr"/>
       <c r="K186" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="L186" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="M186" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="N186" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="O186" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="L186" t="inlineStr"/>
+      <c r="M186" t="inlineStr"/>
+      <c r="N186" t="inlineStr"/>
+      <c r="O186" t="inlineStr"/>
       <c r="P186" t="inlineStr">
         <is>
           <t>x</t>
@@ -14570,12 +14550,12 @@
       <c r="U186" t="inlineStr"/>
       <c r="V186" t="inlineStr">
         <is>
-          <t>FlHcvD</t>
+          <t>AvO75HcvD</t>
         </is>
       </c>
       <c r="W186" t="inlineStr">
         <is>
-          <t>Hepatitis C Deaths - Women</t>
+          <t>Hepatitis C Deaths - Age Over 75  (5-Year Averages)</t>
         </is>
       </c>
       <c r="X186" t="inlineStr"/>
@@ -14626,7 +14606,11 @@
       <c r="M187" t="inlineStr"/>
       <c r="N187" t="inlineStr"/>
       <c r="O187" t="inlineStr"/>
-      <c r="P187" t="inlineStr"/>
+      <c r="P187" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q187" t="inlineStr"/>
       <c r="R187" t="inlineStr"/>
       <c r="S187" t="inlineStr"/>
@@ -14634,12 +14618,12 @@
       <c r="U187" t="inlineStr"/>
       <c r="V187" t="inlineStr">
         <is>
-          <t>FmHcv</t>
+          <t>AvU50HcvD</t>
         </is>
       </c>
       <c r="W187" t="inlineStr">
         <is>
-          <t>Yearly Hepatitis C cases - Women (2013-2016)</t>
+          <t>Hepatitis C Deaths - Age Under 50 (5-Year Averages)</t>
         </is>
       </c>
       <c r="X187" t="inlineStr"/>
@@ -14677,51 +14661,15 @@
       <c r="D188" t="inlineStr"/>
       <c r="E188" t="inlineStr"/>
       <c r="F188" t="inlineStr"/>
-      <c r="G188" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="H188" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="I188" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="J188" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="K188" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="L188" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="M188" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="N188" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="O188" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="G188" t="inlineStr"/>
+      <c r="H188" t="inlineStr"/>
+      <c r="I188" t="inlineStr"/>
+      <c r="J188" t="inlineStr"/>
+      <c r="K188" t="inlineStr"/>
+      <c r="L188" t="inlineStr"/>
+      <c r="M188" t="inlineStr"/>
+      <c r="N188" t="inlineStr"/>
+      <c r="O188" t="inlineStr"/>
       <c r="P188" t="inlineStr">
         <is>
           <t>x</t>
@@ -14734,12 +14682,12 @@
       <c r="U188" t="inlineStr"/>
       <c r="V188" t="inlineStr">
         <is>
-          <t>HcvD</t>
+          <t>AvWhHcvD</t>
         </is>
       </c>
       <c r="W188" t="inlineStr">
         <is>
-          <t>Hepatitis C Deaths</t>
+          <t>Average White Hepitatis C virus Deaths</t>
         </is>
       </c>
       <c r="X188" t="inlineStr"/>
@@ -14777,56 +14725,20 @@
       <c r="D189" t="inlineStr"/>
       <c r="E189" t="inlineStr"/>
       <c r="F189" t="inlineStr"/>
-      <c r="G189" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="H189" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="I189" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="J189" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="G189" t="inlineStr"/>
+      <c r="H189" t="inlineStr"/>
+      <c r="I189" t="inlineStr"/>
+      <c r="J189" t="inlineStr"/>
       <c r="K189" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="L189" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="M189" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="N189" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="O189" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="P189" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="L189" t="inlineStr"/>
+      <c r="M189" t="inlineStr"/>
+      <c r="N189" t="inlineStr"/>
+      <c r="O189" t="inlineStr"/>
+      <c r="P189" t="inlineStr"/>
       <c r="Q189" t="inlineStr"/>
       <c r="R189" t="inlineStr"/>
       <c r="S189" t="inlineStr"/>
@@ -14834,12 +14746,12 @@
       <c r="U189" t="inlineStr"/>
       <c r="V189" t="inlineStr">
         <is>
-          <t>HspHcvD</t>
+          <t>BlkHcv</t>
         </is>
       </c>
       <c r="W189" t="inlineStr">
         <is>
-          <t>Hepatitis C Deaths - Hispanic</t>
+          <t>Yearly Hepatitis C cases - Black (2013-2016)</t>
         </is>
       </c>
       <c r="X189" t="inlineStr"/>
@@ -14877,20 +14789,56 @@
       <c r="D190" t="inlineStr"/>
       <c r="E190" t="inlineStr"/>
       <c r="F190" t="inlineStr"/>
-      <c r="G190" t="inlineStr"/>
-      <c r="H190" t="inlineStr"/>
-      <c r="I190" t="inlineStr"/>
-      <c r="J190" t="inlineStr"/>
+      <c r="G190" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H190" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="I190" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="J190" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="K190" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="L190" t="inlineStr"/>
-      <c r="M190" t="inlineStr"/>
-      <c r="N190" t="inlineStr"/>
-      <c r="O190" t="inlineStr"/>
-      <c r="P190" t="inlineStr"/>
+      <c r="L190" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="M190" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="N190" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="O190" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="P190" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q190" t="inlineStr"/>
       <c r="R190" t="inlineStr"/>
       <c r="S190" t="inlineStr"/>
@@ -14898,12 +14846,12 @@
       <c r="U190" t="inlineStr"/>
       <c r="V190" t="inlineStr">
         <is>
-          <t>MlHcv</t>
+          <t>BlkHcvD</t>
         </is>
       </c>
       <c r="W190" t="inlineStr">
         <is>
-          <t>Yearly Hepatitis C cases - Men (2013-2016)</t>
+          <t>Hepatitis C Deaths - Black</t>
         </is>
       </c>
       <c r="X190" t="inlineStr"/>
@@ -14998,12 +14946,12 @@
       <c r="U191" t="inlineStr"/>
       <c r="V191" t="inlineStr">
         <is>
-          <t>MlHcvD</t>
+          <t>FlHcvD</t>
         </is>
       </c>
       <c r="W191" t="inlineStr">
         <is>
-          <t>Hepatitis C Deaths - Men</t>
+          <t>Hepatitis C Deaths - Women</t>
         </is>
       </c>
       <c r="X191" t="inlineStr"/>
@@ -15045,32 +14993,16 @@
       <c r="H192" t="inlineStr"/>
       <c r="I192" t="inlineStr"/>
       <c r="J192" t="inlineStr"/>
-      <c r="K192" t="inlineStr"/>
-      <c r="L192" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="M192" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="N192" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="O192" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="P192" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K192" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="L192" t="inlineStr"/>
+      <c r="M192" t="inlineStr"/>
+      <c r="N192" t="inlineStr"/>
+      <c r="O192" t="inlineStr"/>
+      <c r="P192" t="inlineStr"/>
       <c r="Q192" t="inlineStr"/>
       <c r="R192" t="inlineStr"/>
       <c r="S192" t="inlineStr"/>
@@ -15078,12 +15010,12 @@
       <c r="U192" t="inlineStr"/>
       <c r="V192" t="inlineStr">
         <is>
-          <t>MulHcvD</t>
+          <t>FmHcv</t>
         </is>
       </c>
       <c r="W192" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hepatitis C deaths among Multiple Race populations </t>
+          <t>Yearly Hepatitis C cases - Women (2013-2016)</t>
         </is>
       </c>
       <c r="X192" t="inlineStr"/>
@@ -15121,11 +15053,31 @@
       <c r="D193" t="inlineStr"/>
       <c r="E193" t="inlineStr"/>
       <c r="F193" t="inlineStr"/>
-      <c r="G193" t="inlineStr"/>
-      <c r="H193" t="inlineStr"/>
-      <c r="I193" t="inlineStr"/>
-      <c r="J193" t="inlineStr"/>
-      <c r="K193" t="inlineStr"/>
+      <c r="G193" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H193" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="I193" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="J193" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="K193" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L193" t="inlineStr">
         <is>
           <t>x</t>
@@ -15158,12 +15110,12 @@
       <c r="U193" t="inlineStr"/>
       <c r="V193" t="inlineStr">
         <is>
-          <t>NhPiHcvD</t>
+          <t>HcvD</t>
         </is>
       </c>
       <c r="W193" t="inlineStr">
         <is>
-          <t xml:space="preserve">Hepatitis C deaths among Native Hawaiian and Pacific Islander populations </t>
+          <t>Hepatitis C Deaths</t>
         </is>
       </c>
       <c r="X193" t="inlineStr"/>
@@ -15201,20 +15153,56 @@
       <c r="D194" t="inlineStr"/>
       <c r="E194" t="inlineStr"/>
       <c r="F194" t="inlineStr"/>
-      <c r="G194" t="inlineStr"/>
-      <c r="H194" t="inlineStr"/>
-      <c r="I194" t="inlineStr"/>
-      <c r="J194" t="inlineStr"/>
+      <c r="G194" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H194" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="I194" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="J194" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="K194" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="L194" t="inlineStr"/>
-      <c r="M194" t="inlineStr"/>
-      <c r="N194" t="inlineStr"/>
-      <c r="O194" t="inlineStr"/>
-      <c r="P194" t="inlineStr"/>
+      <c r="L194" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="M194" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="N194" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="O194" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="P194" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q194" t="inlineStr"/>
       <c r="R194" t="inlineStr"/>
       <c r="S194" t="inlineStr"/>
@@ -15222,12 +15210,12 @@
       <c r="U194" t="inlineStr"/>
       <c r="V194" t="inlineStr">
         <is>
-          <t>NonBlkHcv</t>
+          <t>HspHcvD</t>
         </is>
       </c>
       <c r="W194" t="inlineStr">
         <is>
-          <t>Yearly Hepatitis C cases - non-Black (2013-2016)</t>
+          <t>Hepatitis C Deaths - Hispanic</t>
         </is>
       </c>
       <c r="X194" t="inlineStr"/>
@@ -15265,56 +15253,20 @@
       <c r="D195" t="inlineStr"/>
       <c r="E195" t="inlineStr"/>
       <c r="F195" t="inlineStr"/>
-      <c r="G195" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="H195" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="I195" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="J195" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="G195" t="inlineStr"/>
+      <c r="H195" t="inlineStr"/>
+      <c r="I195" t="inlineStr"/>
+      <c r="J195" t="inlineStr"/>
       <c r="K195" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="L195" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="M195" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="N195" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="O195" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="P195" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="L195" t="inlineStr"/>
+      <c r="M195" t="inlineStr"/>
+      <c r="N195" t="inlineStr"/>
+      <c r="O195" t="inlineStr"/>
+      <c r="P195" t="inlineStr"/>
       <c r="Q195" t="inlineStr"/>
       <c r="R195" t="inlineStr"/>
       <c r="S195" t="inlineStr"/>
@@ -15322,12 +15274,12 @@
       <c r="U195" t="inlineStr"/>
       <c r="V195" t="inlineStr">
         <is>
-          <t>O75HcvD</t>
+          <t>MlHcv</t>
         </is>
       </c>
       <c r="W195" t="inlineStr">
         <is>
-          <t>Hepatitis C Deaths - Over 75 years old</t>
+          <t>Yearly Hepatitis C cases - Men (2013-2016)</t>
         </is>
       </c>
       <c r="X195" t="inlineStr"/>
@@ -15365,20 +15317,56 @@
       <c r="D196" t="inlineStr"/>
       <c r="E196" t="inlineStr"/>
       <c r="F196" t="inlineStr"/>
-      <c r="G196" t="inlineStr"/>
-      <c r="H196" t="inlineStr"/>
-      <c r="I196" t="inlineStr"/>
-      <c r="J196" t="inlineStr"/>
+      <c r="G196" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H196" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="I196" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="J196" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="K196" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="L196" t="inlineStr"/>
-      <c r="M196" t="inlineStr"/>
-      <c r="N196" t="inlineStr"/>
-      <c r="O196" t="inlineStr"/>
-      <c r="P196" t="inlineStr"/>
+      <c r="L196" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="M196" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="N196" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="O196" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="P196" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q196" t="inlineStr"/>
       <c r="R196" t="inlineStr"/>
       <c r="S196" t="inlineStr"/>
@@ -15386,12 +15374,12 @@
       <c r="U196" t="inlineStr"/>
       <c r="V196" t="inlineStr">
         <is>
-          <t>Ov75Hcv</t>
+          <t>MlHcvD</t>
         </is>
       </c>
       <c r="W196" t="inlineStr">
         <is>
-          <t>Yearly Hepatitis C cases - Over 75 years old (2013-2016)</t>
+          <t>Hepatitis C Deaths - Men</t>
         </is>
       </c>
       <c r="X196" t="inlineStr"/>
@@ -15433,16 +15421,32 @@
       <c r="H197" t="inlineStr"/>
       <c r="I197" t="inlineStr"/>
       <c r="J197" t="inlineStr"/>
-      <c r="K197" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="L197" t="inlineStr"/>
-      <c r="M197" t="inlineStr"/>
-      <c r="N197" t="inlineStr"/>
-      <c r="O197" t="inlineStr"/>
-      <c r="P197" t="inlineStr"/>
+      <c r="K197" t="inlineStr"/>
+      <c r="L197" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="M197" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="N197" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="O197" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="P197" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Q197" t="inlineStr"/>
       <c r="R197" t="inlineStr"/>
       <c r="S197" t="inlineStr"/>
@@ -15450,12 +15454,12 @@
       <c r="U197" t="inlineStr"/>
       <c r="V197" t="inlineStr">
         <is>
-          <t>TotHcv</t>
+          <t>MulHcvD</t>
         </is>
       </c>
       <c r="W197" t="inlineStr">
         <is>
-          <t>Yearly Hepatitis C cases (2013-2016)</t>
+          <t xml:space="preserve">Hepatitis C deaths among Multiple Race populations </t>
         </is>
       </c>
       <c r="X197" t="inlineStr"/>
@@ -15493,31 +15497,11 @@
       <c r="D198" t="inlineStr"/>
       <c r="E198" t="inlineStr"/>
       <c r="F198" t="inlineStr"/>
-      <c r="G198" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="H198" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="I198" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="J198" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="K198" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="G198" t="inlineStr"/>
+      <c r="H198" t="inlineStr"/>
+      <c r="I198" t="inlineStr"/>
+      <c r="J198" t="inlineStr"/>
+      <c r="K198" t="inlineStr"/>
       <c r="L198" t="inlineStr">
         <is>
           <t>x</t>
@@ -15550,12 +15534,12 @@
       <c r="U198" t="inlineStr"/>
       <c r="V198" t="inlineStr">
         <is>
-          <t>U50HcvD</t>
+          <t>NhPiHcvD</t>
         </is>
       </c>
       <c r="W198" t="inlineStr">
         <is>
-          <t>Hepatitis C Deaths - Under 50 years old</t>
+          <t xml:space="preserve">Hepatitis C deaths among Native Hawaiian and Pacific Islander populations </t>
         </is>
       </c>
       <c r="X198" t="inlineStr"/>
@@ -15614,12 +15598,12 @@
       <c r="U199" t="inlineStr"/>
       <c r="V199" t="inlineStr">
         <is>
-          <t>Un50Hcv</t>
+          <t>NonBlkHcv</t>
         </is>
       </c>
       <c r="W199" t="inlineStr">
         <is>
-          <t>Yearly Hepatitis C cases - Under 50 years old (2013-2016)</t>
+          <t>Yearly Hepatitis C cases - non-Black (2013-2016)</t>
         </is>
       </c>
       <c r="X199" t="inlineStr"/>
@@ -15657,11 +15641,31 @@
       <c r="D200" t="inlineStr"/>
       <c r="E200" t="inlineStr"/>
       <c r="F200" t="inlineStr"/>
-      <c r="G200" t="inlineStr"/>
-      <c r="H200" t="inlineStr"/>
-      <c r="I200" t="inlineStr"/>
-      <c r="J200" t="inlineStr"/>
-      <c r="K200" t="inlineStr"/>
+      <c r="G200" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H200" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="I200" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="J200" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="K200" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L200" t="inlineStr">
         <is>
           <t>x</t>
@@ -15694,12 +15698,12 @@
       <c r="U200" t="inlineStr"/>
       <c r="V200" t="inlineStr">
         <is>
-          <t>WhtHcvD</t>
+          <t>O75HcvD</t>
         </is>
       </c>
       <c r="W200" t="inlineStr">
         <is>
-          <t>Hepatitis C deaths among White populations</t>
+          <t>Hepatitis C Deaths - Over 75 years old</t>
         </is>
       </c>
       <c r="X200" t="inlineStr"/>
@@ -15730,7 +15734,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Opioid Indicators</t>
+          <t>Hepatitis C Rates</t>
         </is>
       </c>
       <c r="C201" t="inlineStr"/>
@@ -15738,51 +15742,19 @@
       <c r="E201" t="inlineStr"/>
       <c r="F201" t="inlineStr"/>
       <c r="G201" t="inlineStr"/>
-      <c r="H201" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="I201" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="J201" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="H201" t="inlineStr"/>
+      <c r="I201" t="inlineStr"/>
+      <c r="J201" t="inlineStr"/>
       <c r="K201" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="L201" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="M201" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="N201" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="O201" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="P201" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="L201" t="inlineStr"/>
+      <c r="M201" t="inlineStr"/>
+      <c r="N201" t="inlineStr"/>
+      <c r="O201" t="inlineStr"/>
+      <c r="P201" t="inlineStr"/>
       <c r="Q201" t="inlineStr"/>
       <c r="R201" t="inlineStr"/>
       <c r="S201" t="inlineStr"/>
@@ -15790,28 +15762,28 @@
       <c r="U201" t="inlineStr"/>
       <c r="V201" t="inlineStr">
         <is>
-          <t>OdMortRt</t>
+          <t>Ov75Hcv</t>
         </is>
       </c>
       <c r="W201" t="inlineStr">
         <is>
-          <t>Overdose Mortality Rate</t>
+          <t>Yearly Hepatitis C cases - Over 75 years old (2013-2016)</t>
         </is>
       </c>
       <c r="X201" t="inlineStr"/>
       <c r="Y201" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Opioid_Outcomes.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/HepatitisC_Rates.md</t>
         </is>
       </c>
       <c r="Z201" t="inlineStr">
         <is>
-          <t>HepVu 2014-2022</t>
+          <t>HepVu 2013-2016, 2018-2022</t>
         </is>
       </c>
       <c r="AA201" t="inlineStr">
         <is>
-          <t>HepVu, Emory University Rollins School of Public Health, 2014-2022</t>
+          <t>HepVu, Emory University Rollins School of Public Health, 2013-2016 &amp; 2018-2022</t>
         </is>
       </c>
       <c r="AB201" t="inlineStr"/>
@@ -15826,7 +15798,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Opioid Indicators</t>
+          <t>Hepatitis C Rates</t>
         </is>
       </c>
       <c r="C202" t="inlineStr"/>
@@ -15837,14 +15809,14 @@
       <c r="H202" t="inlineStr"/>
       <c r="I202" t="inlineStr"/>
       <c r="J202" t="inlineStr"/>
-      <c r="K202" t="inlineStr"/>
+      <c r="K202" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L202" t="inlineStr"/>
       <c r="M202" t="inlineStr"/>
-      <c r="N202" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="N202" t="inlineStr"/>
       <c r="O202" t="inlineStr"/>
       <c r="P202" t="inlineStr"/>
       <c r="Q202" t="inlineStr"/>
@@ -15854,28 +15826,28 @@
       <c r="U202" t="inlineStr"/>
       <c r="V202" t="inlineStr">
         <is>
-          <t>OdMortRtAv</t>
+          <t>TotHcv</t>
         </is>
       </c>
       <c r="W202" t="inlineStr">
         <is>
-          <t>Overdose Mortality Rate Average (2016-2020)</t>
+          <t>Yearly Hepatitis C cases (2013-2016)</t>
         </is>
       </c>
       <c r="X202" t="inlineStr"/>
       <c r="Y202" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Opioid_Outcomes.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/HepatitisC_Rates.md</t>
         </is>
       </c>
       <c r="Z202" t="inlineStr">
         <is>
-          <t>HepVu 2014-2022</t>
+          <t>HepVu 2013-2016, 2018-2022</t>
         </is>
       </c>
       <c r="AA202" t="inlineStr">
         <is>
-          <t>HepVu, Emory University Rollins School of Public Health, 2014-2022</t>
+          <t>HepVu, Emory University Rollins School of Public Health, 2013-2016 &amp; 2018-2022</t>
         </is>
       </c>
       <c r="AB202" t="inlineStr"/>
@@ -15890,26 +15862,58 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Opioid Indicators</t>
+          <t>Hepatitis C Rates</t>
         </is>
       </c>
       <c r="C203" t="inlineStr"/>
       <c r="D203" t="inlineStr"/>
       <c r="E203" t="inlineStr"/>
       <c r="F203" t="inlineStr"/>
-      <c r="G203" t="inlineStr"/>
-      <c r="H203" t="inlineStr"/>
-      <c r="I203" t="inlineStr"/>
-      <c r="J203" t="inlineStr"/>
-      <c r="K203" t="inlineStr"/>
-      <c r="L203" t="inlineStr"/>
-      <c r="M203" t="inlineStr"/>
+      <c r="G203" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H203" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="I203" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="J203" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="K203" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="L203" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="M203" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="N203" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="O203" t="inlineStr"/>
+      <c r="O203" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="P203" t="inlineStr">
         <is>
           <t>x</t>
@@ -15922,28 +15926,28 @@
       <c r="U203" t="inlineStr"/>
       <c r="V203" t="inlineStr">
         <is>
-          <t>OpRxRt</t>
+          <t>U50HcvD</t>
         </is>
       </c>
       <c r="W203" t="inlineStr">
         <is>
-          <t>Opioid Prescription Rate</t>
+          <t>Hepatitis C Deaths - Under 50 years old</t>
         </is>
       </c>
       <c r="X203" t="inlineStr"/>
       <c r="Y203" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Opioid_Outcomes.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/HepatitisC_Rates.md</t>
         </is>
       </c>
       <c r="Z203" t="inlineStr">
         <is>
-          <t>HepVu 2014-2022</t>
+          <t>HepVu 2013-2016, 2018-2022</t>
         </is>
       </c>
       <c r="AA203" t="inlineStr">
         <is>
-          <t>HepVu, Emory University Rollins School of Public Health, 2014-2022</t>
+          <t>HepVu, Emory University Rollins School of Public Health, 2013-2016 &amp; 2018-2022</t>
         </is>
       </c>
       <c r="AB203" t="inlineStr"/>
@@ -15958,7 +15962,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Opioid Indicators</t>
+          <t>Hepatitis C Rates</t>
         </is>
       </c>
       <c r="C204" t="inlineStr"/>
@@ -15969,20 +15973,16 @@
       <c r="H204" t="inlineStr"/>
       <c r="I204" t="inlineStr"/>
       <c r="J204" t="inlineStr"/>
-      <c r="K204" t="inlineStr"/>
+      <c r="K204" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="L204" t="inlineStr"/>
       <c r="M204" t="inlineStr"/>
-      <c r="N204" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="N204" t="inlineStr"/>
       <c r="O204" t="inlineStr"/>
-      <c r="P204" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P204" t="inlineStr"/>
       <c r="Q204" t="inlineStr"/>
       <c r="R204" t="inlineStr"/>
       <c r="S204" t="inlineStr"/>
@@ -15990,33 +15990,409 @@
       <c r="U204" t="inlineStr"/>
       <c r="V204" t="inlineStr">
         <is>
-          <t>PrMsuseP</t>
+          <t>Un50Hcv</t>
         </is>
       </c>
       <c r="W204" t="inlineStr">
         <is>
-          <t>% Self-Report Misuse of Prescription Pain Medication (2020)</t>
+          <t>Yearly Hepatitis C cases - Under 50 years old (2013-2016)</t>
         </is>
       </c>
       <c r="X204" t="inlineStr"/>
       <c r="Y204" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Opioid_Outcomes.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/HepatitisC_Rates.md</t>
         </is>
       </c>
       <c r="Z204" t="inlineStr">
         <is>
-          <t>HepVu 2014-2022</t>
+          <t>HepVu 2013-2016, 2018-2022</t>
         </is>
       </c>
       <c r="AA204" t="inlineStr">
         <is>
-          <t>HepVu, Emory University Rollins School of Public Health, 2014-2022</t>
+          <t>HepVu, Emory University Rollins School of Public Health, 2013-2016 &amp; 2018-2022</t>
         </is>
       </c>
       <c r="AB204" t="inlineStr"/>
       <c r="AC204" t="inlineStr"/>
       <c r="AD204" t="inlineStr"/>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>Outcome</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>Hepatitis C Rates</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr"/>
+      <c r="D205" t="inlineStr"/>
+      <c r="E205" t="inlineStr"/>
+      <c r="F205" t="inlineStr"/>
+      <c r="G205" t="inlineStr"/>
+      <c r="H205" t="inlineStr"/>
+      <c r="I205" t="inlineStr"/>
+      <c r="J205" t="inlineStr"/>
+      <c r="K205" t="inlineStr"/>
+      <c r="L205" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="M205" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="N205" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="O205" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="P205" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="Q205" t="inlineStr"/>
+      <c r="R205" t="inlineStr"/>
+      <c r="S205" t="inlineStr"/>
+      <c r="T205" t="inlineStr"/>
+      <c r="U205" t="inlineStr"/>
+      <c r="V205" t="inlineStr">
+        <is>
+          <t>WhtHcvD</t>
+        </is>
+      </c>
+      <c r="W205" t="inlineStr">
+        <is>
+          <t>Hepatitis C deaths among White populations</t>
+        </is>
+      </c>
+      <c r="X205" t="inlineStr"/>
+      <c r="Y205" t="inlineStr">
+        <is>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/HepatitisC_Rates.md</t>
+        </is>
+      </c>
+      <c r="Z205" t="inlineStr">
+        <is>
+          <t>HepVu 2013-2016, 2018-2022</t>
+        </is>
+      </c>
+      <c r="AA205" t="inlineStr">
+        <is>
+          <t>HepVu, Emory University Rollins School of Public Health, 2013-2016 &amp; 2018-2022</t>
+        </is>
+      </c>
+      <c r="AB205" t="inlineStr"/>
+      <c r="AC205" t="inlineStr"/>
+      <c r="AD205" t="inlineStr"/>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>Outcome</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>Opioid Indicators</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr"/>
+      <c r="D206" t="inlineStr"/>
+      <c r="E206" t="inlineStr"/>
+      <c r="F206" t="inlineStr"/>
+      <c r="G206" t="inlineStr"/>
+      <c r="H206" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="I206" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="J206" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="K206" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="L206" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="M206" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="N206" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="O206" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="P206" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="Q206" t="inlineStr"/>
+      <c r="R206" t="inlineStr"/>
+      <c r="S206" t="inlineStr"/>
+      <c r="T206" t="inlineStr"/>
+      <c r="U206" t="inlineStr"/>
+      <c r="V206" t="inlineStr">
+        <is>
+          <t>OdMortRt</t>
+        </is>
+      </c>
+      <c r="W206" t="inlineStr">
+        <is>
+          <t>Overdose Mortality Rate</t>
+        </is>
+      </c>
+      <c r="X206" t="inlineStr"/>
+      <c r="Y206" t="inlineStr">
+        <is>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Opioid_Outcomes.md</t>
+        </is>
+      </c>
+      <c r="Z206" t="inlineStr">
+        <is>
+          <t>HepVu 2014-2022</t>
+        </is>
+      </c>
+      <c r="AA206" t="inlineStr">
+        <is>
+          <t>HepVu, Emory University Rollins School of Public Health, 2014-2022</t>
+        </is>
+      </c>
+      <c r="AB206" t="inlineStr"/>
+      <c r="AC206" t="inlineStr"/>
+      <c r="AD206" t="inlineStr"/>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>Outcome</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>Opioid Indicators</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr"/>
+      <c r="D207" t="inlineStr"/>
+      <c r="E207" t="inlineStr"/>
+      <c r="F207" t="inlineStr"/>
+      <c r="G207" t="inlineStr"/>
+      <c r="H207" t="inlineStr"/>
+      <c r="I207" t="inlineStr"/>
+      <c r="J207" t="inlineStr"/>
+      <c r="K207" t="inlineStr"/>
+      <c r="L207" t="inlineStr"/>
+      <c r="M207" t="inlineStr"/>
+      <c r="N207" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="O207" t="inlineStr"/>
+      <c r="P207" t="inlineStr"/>
+      <c r="Q207" t="inlineStr"/>
+      <c r="R207" t="inlineStr"/>
+      <c r="S207" t="inlineStr"/>
+      <c r="T207" t="inlineStr"/>
+      <c r="U207" t="inlineStr"/>
+      <c r="V207" t="inlineStr">
+        <is>
+          <t>OdMortRtAv</t>
+        </is>
+      </c>
+      <c r="W207" t="inlineStr">
+        <is>
+          <t>Overdose Mortality Rate Average (2016-2020)</t>
+        </is>
+      </c>
+      <c r="X207" t="inlineStr"/>
+      <c r="Y207" t="inlineStr">
+        <is>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Opioid_Outcomes.md</t>
+        </is>
+      </c>
+      <c r="Z207" t="inlineStr">
+        <is>
+          <t>HepVu 2014-2022</t>
+        </is>
+      </c>
+      <c r="AA207" t="inlineStr">
+        <is>
+          <t>HepVu, Emory University Rollins School of Public Health, 2014-2022</t>
+        </is>
+      </c>
+      <c r="AB207" t="inlineStr"/>
+      <c r="AC207" t="inlineStr"/>
+      <c r="AD207" t="inlineStr"/>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>Outcome</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>Opioid Indicators</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr"/>
+      <c r="D208" t="inlineStr"/>
+      <c r="E208" t="inlineStr"/>
+      <c r="F208" t="inlineStr"/>
+      <c r="G208" t="inlineStr"/>
+      <c r="H208" t="inlineStr"/>
+      <c r="I208" t="inlineStr"/>
+      <c r="J208" t="inlineStr"/>
+      <c r="K208" t="inlineStr"/>
+      <c r="L208" t="inlineStr"/>
+      <c r="M208" t="inlineStr"/>
+      <c r="N208" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="O208" t="inlineStr"/>
+      <c r="P208" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="Q208" t="inlineStr"/>
+      <c r="R208" t="inlineStr"/>
+      <c r="S208" t="inlineStr"/>
+      <c r="T208" t="inlineStr"/>
+      <c r="U208" t="inlineStr"/>
+      <c r="V208" t="inlineStr">
+        <is>
+          <t>OpRxRt</t>
+        </is>
+      </c>
+      <c r="W208" t="inlineStr">
+        <is>
+          <t>Opioid Prescription Rate</t>
+        </is>
+      </c>
+      <c r="X208" t="inlineStr"/>
+      <c r="Y208" t="inlineStr">
+        <is>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Opioid_Outcomes.md</t>
+        </is>
+      </c>
+      <c r="Z208" t="inlineStr">
+        <is>
+          <t>HepVu 2014-2022</t>
+        </is>
+      </c>
+      <c r="AA208" t="inlineStr">
+        <is>
+          <t>HepVu, Emory University Rollins School of Public Health, 2014-2022</t>
+        </is>
+      </c>
+      <c r="AB208" t="inlineStr"/>
+      <c r="AC208" t="inlineStr"/>
+      <c r="AD208" t="inlineStr"/>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>Outcome</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Opioid Indicators</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr"/>
+      <c r="D209" t="inlineStr"/>
+      <c r="E209" t="inlineStr"/>
+      <c r="F209" t="inlineStr"/>
+      <c r="G209" t="inlineStr"/>
+      <c r="H209" t="inlineStr"/>
+      <c r="I209" t="inlineStr"/>
+      <c r="J209" t="inlineStr"/>
+      <c r="K209" t="inlineStr"/>
+      <c r="L209" t="inlineStr"/>
+      <c r="M209" t="inlineStr"/>
+      <c r="N209" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="O209" t="inlineStr"/>
+      <c r="P209" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="Q209" t="inlineStr"/>
+      <c r="R209" t="inlineStr"/>
+      <c r="S209" t="inlineStr"/>
+      <c r="T209" t="inlineStr"/>
+      <c r="U209" t="inlineStr"/>
+      <c r="V209" t="inlineStr">
+        <is>
+          <t>PrMsuseP</t>
+        </is>
+      </c>
+      <c r="W209" t="inlineStr">
+        <is>
+          <t>% Self-Report Misuse of Prescription Pain Medication (2020)</t>
+        </is>
+      </c>
+      <c r="X209" t="inlineStr"/>
+      <c r="Y209" t="inlineStr">
+        <is>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Opioid_Outcomes.md</t>
+        </is>
+      </c>
+      <c r="Z209" t="inlineStr">
+        <is>
+          <t>HepVu 2014-2022</t>
+        </is>
+      </c>
+      <c r="AA209" t="inlineStr">
+        <is>
+          <t>HepVu, Emory University Rollins School of Public Health, 2014-2022</t>
+        </is>
+      </c>
+      <c r="AB209" t="inlineStr"/>
+      <c r="AC209" t="inlineStr"/>
+      <c r="AD209" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>